<commit_message>
Updated BOM status for latest purchases
</commit_message>
<xml_diff>
--- a/BOM/voron2.4_350mm_bom.xlsx
+++ b/BOM/voron2.4_350mm_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cwilder/Documents/3D Printing/cee-wals/voron-2.4/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F0706B-24D2-6D4B-A043-4E37FC11F7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0FBAE9-24A6-CE44-830F-B6FCAA28012E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="3460" windowWidth="38640" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="500" windowWidth="50420" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="West3D Voron 2.4 BOM" sheetId="6" r:id="rId1"/>
@@ -929,7 +929,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1690" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="502">
   <si>
     <t>Category</t>
   </si>
@@ -2331,9 +2331,6 @@
     <t>Partial Order</t>
   </si>
   <si>
-    <t>Voron Txn 1 (TWW-KF-VORON-1) TWW Kids fund (proj. voron): $146.82 on 10/24/2022</t>
-  </si>
-  <si>
     <t>Cost Adjustments</t>
   </si>
   <si>
@@ -2356,9 +2353,6 @@
   </si>
   <si>
     <t>1 for Voron. 1 for private stock</t>
-  </si>
-  <si>
-    <t>Voron Txn 3 (TWW-KF-VORON-3) TWW Kids fund (proj. voron): $530.90 on 11/11/2022</t>
   </si>
   <si>
     <t>TWW-KF-VORON-3
@@ -2402,14 +2396,7 @@
 Direct from TWW account</t>
   </si>
   <si>
-    <t>Voron Txn 4 (TWW-KF-VORON-4) TWW Kids fund (proj. voron): $543.42 on 12/02/2022</t>
-  </si>
-  <si>
     <t>Accidentally bought the Z PCB. I originally planned on buying the Omron Mouse Button</t>
-  </si>
-  <si>
-    <t>Voron Txn 1 (TWW-KF-VORON-1) TWW Kids fund (proj. voron): $71.98 on 10/07/2022
-Voron Txn 5 (TWW-KF-VORON-5) TWW Kids fund (proj. voron): $136.98 on 12/02/2022</t>
   </si>
   <si>
     <t>TWW-KF-VORON-1
@@ -2427,9 +2414,6 @@
     <t>Mandala Roseworks Matched height kinematic kit</t>
   </si>
   <si>
-    <t>Voron Txn 6 (TWW-KF-VORON-6) TWW Kids fund (proj. voron): $131.12 on 12/05/2022</t>
-  </si>
-  <si>
     <t>TWW-KF-VORON-6
 Direct from TWW account</t>
   </si>
@@ -2440,9 +2424,6 @@
     <t>Mandala Roseworks The "Gripper" E3DV6 Wrench</t>
   </si>
   <si>
-    <t>Voron Txn 7 (TWW-KF-VORON-7) TWW Kids fund (proj. voron): $35.27 on 12/05/2022</t>
-  </si>
-  <si>
     <t>Layerneer Bed Weld - Original 3D printing adhesive</t>
   </si>
   <si>
@@ -2453,22 +2434,105 @@
 Purchase through Mandala Roseworks - Shop store</t>
   </si>
   <si>
-    <t>Shipping is split between orders.
-Purchase through Mandala Roseworks - Shop store</t>
-  </si>
-  <si>
-    <t>Purchase through Mandala Roseworks - Shop store</t>
-  </si>
-  <si>
-    <t>Voron Txn 8 (TWW-KF-VORON-8) TWW Kids fund (proj. voron): $22.95 on 12/05/2022</t>
-  </si>
-  <si>
     <t>TWW-KF-VORON-7
 Direct from TWW account</t>
   </si>
   <si>
     <t>TWW-KF-VORON-8
 Direct from TWW account</t>
+  </si>
+  <si>
+    <t>Voron Tap - rail w/ optotap v2 (5-24v) and HW kit; from DFH</t>
+  </si>
+  <si>
+    <t>Not required but highly recommended
+Shipping is split between orders.
+Purchased from Mandala Roseworks - Shop store</t>
+  </si>
+  <si>
+    <t>Nightlight on a stick - LED Strip; from DFH</t>
+  </si>
+  <si>
+    <t>Disco stick on black PCB - LED Strip; from DFH</t>
+  </si>
+  <si>
+    <t>Daylight on a stick on black PCB; from DFH</t>
+  </si>
+  <si>
+    <t>OV5640 Camera Module; from DFH</t>
+  </si>
+  <si>
+    <t>Seeeduino XIAO; from DFH</t>
+  </si>
+  <si>
+    <t>Optional add-on
+Purchased from DFH - Shop store</t>
+  </si>
+  <si>
+    <t>TWW-KF-VORON-9
+Direct from TWW account</t>
+  </si>
+  <si>
+    <t>TWW-KF-VORON-9</t>
+  </si>
+  <si>
+    <t>Bought for other projects
+Purchased from DFH - Shop store</t>
+  </si>
+  <si>
+    <t>Not all for Voron. LED controller and other projects
+Purchased from DFH - Shop store</t>
+  </si>
+  <si>
+    <t>TWW-KF-VORON-2
+Pay Apple CC from TWW account</t>
+  </si>
+  <si>
+    <t>Shipping is split between items. 
+Purchased from DFH - Shop store</t>
+  </si>
+  <si>
+    <t>Shipping is split between items.
+Purchased from Mandala Roseworks - Shop store</t>
+  </si>
+  <si>
+    <t>Voron Txn 7 (TWW-KF-VORON-7)
+TWW Kids fund (proj. voron): $35.27 on 12/05/2022
+total shipping: $6.27</t>
+  </si>
+  <si>
+    <t>Voron Txn 6 (TWW-KF-VORON-6) 
+TWW Kids fund (proj. voron): $131.12 on 12/05/2022
+total shipping: $8.12</t>
+  </si>
+  <si>
+    <t>Voron Txn 1 (TWW-KF-VORON-1)
+TWW Kids fund (proj. voron): $71.98 on 10/07/2022
+Voron Txn 5 (TWW-KF-VORON-5)
+TWW Kids fund (proj. voron): $136.98 on 12/02/2022</t>
+  </si>
+  <si>
+    <t>Voron Txn 8 (TWW-KF-VORON-8)
+TWW Kids fund (proj. voron): $22.95 on 12/05/2022</t>
+  </si>
+  <si>
+    <t>Voron Txn 9 (TWW-KF-VORON-9)
+TWW Kids fund (proj. voron): $182.63 on 12/08/2022
+total shipping: $20.18; total discount: $18.05</t>
+  </si>
+  <si>
+    <t>Voron Txn 2 (TWW-KF-VORON-2)
+TWW Kids fund (proj. voron): $146.82 on 10/24/2022
+total shipping: $41.82</t>
+  </si>
+  <si>
+    <t>Voron Txn 4 (TWW-KF-VORON-4)
+TWW Kids fund (proj. voron): $543.42 on 12/02/2022</t>
+  </si>
+  <si>
+    <t>Voron Txn 3 (TWW-KF-VORON-3)
+TWW Kids fund (proj. voron): $530.90 on 11/11/2022
+total shipping: $10.00</t>
   </si>
 </sst>
 </file>
@@ -3827,6 +3891,9 @@
     <xf numFmtId="0" fontId="45" fillId="39" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3868,9 +3935,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -4276,13 +4340,13 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:AD101"/>
+  <dimension ref="A1:AD111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="L56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="2" topLeftCell="M57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R85" sqref="R85"/>
+      <selection pane="bottomRight" activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4294,7 +4358,7 @@
     <col min="6" max="6" width="21.33203125" style="57" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.1640625" style="57" customWidth="1"/>
     <col min="8" max="8" width="64.5" style="57" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.1640625" style="21" customWidth="1"/>
+    <col min="9" max="9" width="41" style="21" customWidth="1"/>
     <col min="10" max="10" width="10.33203125" style="55" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="33.5" style="56" customWidth="1"/>
     <col min="12" max="12" width="27.1640625" style="56" customWidth="1"/>
@@ -4309,28 +4373,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="24" customHeight="1">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="133" t="s">
         <v>293</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132"/>
-      <c r="L1" s="132"/>
-      <c r="M1" s="132"/>
-      <c r="N1" s="132"/>
-      <c r="O1" s="132"/>
-      <c r="P1" s="132"/>
-      <c r="Q1" s="132"/>
-      <c r="R1" s="132"/>
-      <c r="S1" s="132"/>
-      <c r="T1" s="132"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="133"/>
+      <c r="O1" s="133"/>
+      <c r="P1" s="133"/>
+      <c r="Q1" s="133"/>
+      <c r="R1" s="133"/>
+      <c r="S1" s="133"/>
+      <c r="T1" s="133"/>
     </row>
     <row r="2" spans="1:30" s="92" customFormat="1" ht="23" customHeight="1" thickBot="1">
       <c r="A2" s="93" t="s">
@@ -4382,7 +4446,7 @@
         <v>139</v>
       </c>
       <c r="Q2" s="95" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="R2" s="95" t="s">
         <v>391</v>
@@ -4444,7 +4508,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="34" customHeight="1">
+    <row r="4" spans="1:30" ht="45">
       <c r="A4" s="103" t="s">
         <v>299</v>
       </c>
@@ -4497,10 +4561,10 @@
         <v>392</v>
       </c>
       <c r="S4" s="110" t="s">
-        <v>454</v>
+        <v>501</v>
       </c>
       <c r="T4" s="111" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="AD4" s="87" t="s">
         <v>280</v>
@@ -4531,7 +4595,7 @@
         <v>POWGE Motion Black</v>
       </c>
       <c r="I5" s="122" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J5" s="119">
         <f>B5</f>
@@ -4563,16 +4627,16 @@
         <v>280</v>
       </c>
       <c r="S5" s="125" t="s">
-        <v>468</v>
+        <v>500</v>
       </c>
       <c r="T5" s="126" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="AD5" s="87" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="30">
+    <row r="6" spans="1:30" ht="45">
       <c r="A6" s="103" t="s">
         <v>306</v>
       </c>
@@ -4630,10 +4694,10 @@
         <v>392</v>
       </c>
       <c r="S6" s="110" t="s">
-        <v>445</v>
+        <v>499</v>
       </c>
       <c r="T6" s="111" t="s">
-        <v>281</v>
+        <v>491</v>
       </c>
       <c r="AD6" s="87" t="s">
         <v>392</v>
@@ -4697,10 +4761,10 @@
         <v>392</v>
       </c>
       <c r="S7" s="110" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="T7" s="111" t="s">
-        <v>278</v>
+        <v>491</v>
       </c>
       <c r="AD7" s="87" t="s">
         <v>436</v>
@@ -4725,7 +4789,7 @@
         <v>Updated Rubber Feet for V2.4</v>
       </c>
       <c r="I8" s="122" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="J8" s="119">
         <v>1</v>
@@ -4756,10 +4820,10 @@
         <v>280</v>
       </c>
       <c r="S8" s="125" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="T8" s="126" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="AD8" s="87" t="s">
         <v>443</v>
@@ -4788,7 +4852,7 @@
         <v>Z PCB</v>
       </c>
       <c r="I9" s="122" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="J9" s="119">
         <f t="shared" ref="J9:J23" si="3">B9</f>
@@ -4820,10 +4884,10 @@
         <v>280</v>
       </c>
       <c r="S9" s="125" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="T9" s="126" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="AD9" s="87" t="s">
         <v>444</v>
@@ -4882,10 +4946,10 @@
         <v>280</v>
       </c>
       <c r="S10" s="125" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="T10" s="126" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="AD10" s="88"/>
     </row>
@@ -5070,10 +5134,10 @@
         <v>392</v>
       </c>
       <c r="S14" s="110" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="T14" s="111" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="15" spans="1:30" ht="30">
@@ -5565,10 +5629,10 @@
         <v>392</v>
       </c>
       <c r="S25" s="110" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="T25" s="111" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="26" spans="1:30" ht="30">
@@ -5627,10 +5691,10 @@
         <v>392</v>
       </c>
       <c r="S26" s="110" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="T26" s="111" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="27" spans="1:30" ht="30">
@@ -5689,10 +5753,10 @@
         <v>392</v>
       </c>
       <c r="S27" s="110" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="T27" s="111" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="28" spans="1:30">
@@ -5743,7 +5807,7 @@
     </row>
     <row r="29" spans="1:30" ht="30">
       <c r="A29" s="61" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B29" s="67">
         <v>0</v>
@@ -5753,10 +5817,10 @@
       </c>
       <c r="D29" s="67"/>
       <c r="E29" s="61" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="F29" s="61" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="G29" s="58"/>
       <c r="H29" s="81" t="str">
@@ -5764,7 +5828,7 @@
         <v>Touch Screen 7" PiTFT70 (extra)</v>
       </c>
       <c r="I29" s="76" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="J29" s="63">
         <f t="shared" si="5"/>
@@ -5813,7 +5877,7 @@
         <v>Mini 12864 Display Type B RGB - Choose your color</v>
       </c>
       <c r="I30" s="107" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="J30" s="108">
         <f t="shared" si="5"/>
@@ -5848,10 +5912,10 @@
         <v>392</v>
       </c>
       <c r="S30" s="110" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="T30" s="111" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="31" spans="1:30">
@@ -5903,10 +5967,10 @@
         <v>392</v>
       </c>
       <c r="S31" s="110" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="T31" s="111" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="32" spans="1:30">
@@ -6232,7 +6296,7 @@
         <v>401</v>
       </c>
       <c r="F39" s="118" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G39" s="128"/>
       <c r="H39" s="131" t="str">
@@ -6240,7 +6304,7 @@
         <v>Printed Solide - Aluminum Composite backing Panels</v>
       </c>
       <c r="I39" s="122" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J39" s="119">
         <f t="shared" si="5"/>
@@ -6272,10 +6336,10 @@
         <v>280</v>
       </c>
       <c r="S39" s="125" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="T39" s="126" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="40" spans="1:20" ht="30">
@@ -6377,10 +6441,10 @@
         <v>280</v>
       </c>
       <c r="S41" s="125" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="T41" s="126" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="42" spans="1:20">
@@ -6662,10 +6726,10 @@
         <v>280</v>
       </c>
       <c r="S47" s="125" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="T47" s="126" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="48" spans="1:20">
@@ -6805,10 +6869,10 @@
         <v>280</v>
       </c>
       <c r="S50" s="125" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="T50" s="126" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="51" spans="1:20">
@@ -6860,10 +6924,10 @@
         <v>280</v>
       </c>
       <c r="S51" s="125" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="T51" s="126" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="52" spans="1:20">
@@ -7102,7 +7166,7 @@
         <v>5.99</v>
       </c>
       <c r="L57" s="64">
-        <f t="shared" ref="L57:L82" si="16">J57*K57</f>
+        <f t="shared" ref="L57:L92" si="16">J57*K57</f>
         <v>5.99</v>
       </c>
       <c r="M57" s="64"/>
@@ -7224,7 +7288,7 @@
         <v>424</v>
       </c>
       <c r="J60" s="119">
-        <f t="shared" ref="J60:J82" si="18">B60</f>
+        <f t="shared" ref="J60:J92" si="18">B60</f>
         <v>1</v>
       </c>
       <c r="K60" s="123">
@@ -7253,57 +7317,72 @@
         <v>280</v>
       </c>
       <c r="S60" s="125" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="T60" s="126" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20">
-      <c r="A61" s="61" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" ht="45">
+      <c r="A61" s="118" t="s">
         <v>425</v>
       </c>
-      <c r="B61" s="63">
-        <v>1</v>
-      </c>
-      <c r="C61" s="63" t="s">
+      <c r="B61" s="119">
+        <v>1</v>
+      </c>
+      <c r="C61" s="119" t="s">
         <v>313</v>
       </c>
-      <c r="D61" s="63" t="s">
+      <c r="D61" s="119" t="s">
         <v>298</v>
       </c>
-      <c r="E61" s="65"/>
-      <c r="F61" s="65"/>
-      <c r="G61" s="65"/>
-      <c r="H61" s="68" t="str">
-        <f>A61</f>
-        <v>Kinematics Mount V2.4 (350mm)</v>
-      </c>
-      <c r="I61" s="76" t="s">
-        <v>424</v>
-      </c>
-      <c r="J61" s="63">
+      <c r="E61" s="118" t="s">
+        <v>470</v>
+      </c>
+      <c r="F61" s="120"/>
+      <c r="G61" s="120"/>
+      <c r="H61" s="121" t="str">
+        <f>E61</f>
+        <v>Mandala Roseworks Matched height kinematic kit</v>
+      </c>
+      <c r="I61" s="122" t="s">
+        <v>480</v>
+      </c>
+      <c r="J61" s="119">
         <f t="shared" si="18"/>
         <v>1</v>
       </c>
-      <c r="K61" s="64">
-        <v>84.99</v>
-      </c>
-      <c r="L61" s="64">
+      <c r="K61" s="123">
+        <v>88</v>
+      </c>
+      <c r="L61" s="123">
         <f t="shared" si="16"/>
-        <v>84.99</v>
-      </c>
-      <c r="M61" s="64"/>
-      <c r="N61" s="64"/>
-      <c r="O61" s="64">
+        <v>88</v>
+      </c>
+      <c r="M61" s="123">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="N61" s="123">
+        <v>0</v>
+      </c>
+      <c r="O61" s="123">
         <f t="shared" si="17"/>
-        <v>84.99</v>
-      </c>
-      <c r="P61" s="64"/>
-      <c r="Q61" s="76"/>
-      <c r="R61" s="63"/>
-      <c r="S61" s="99"/>
-      <c r="T61" s="100"/>
+        <v>92.06</v>
+      </c>
+      <c r="P61" s="123">
+        <f>O61</f>
+        <v>92.06</v>
+      </c>
+      <c r="Q61" s="122"/>
+      <c r="R61" s="119" t="s">
+        <v>280</v>
+      </c>
+      <c r="S61" s="125" t="s">
+        <v>472</v>
+      </c>
+      <c r="T61" s="126" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="62" spans="1:20">
       <c r="A62" s="65" t="s">
@@ -7353,7 +7432,7 @@
     </row>
     <row r="63" spans="1:20">
       <c r="A63" s="91" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B63" s="63">
         <v>1</v>
@@ -7436,7 +7515,7 @@
         <v>0</v>
       </c>
       <c r="O64" s="123">
-        <f t="shared" ref="O64:O82" si="20">L64+M64+N64</f>
+        <f t="shared" ref="O64:O92" si="20">L64+M64+N64</f>
         <v>107.97</v>
       </c>
       <c r="P64" s="123">
@@ -7448,10 +7527,10 @@
         <v>280</v>
       </c>
       <c r="S64" s="125" t="s">
-        <v>470</v>
+        <v>496</v>
       </c>
       <c r="T64" s="126" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="65" spans="1:20">
@@ -7513,7 +7592,7 @@
     </row>
     <row r="66" spans="1:20">
       <c r="A66" s="61" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B66" s="63">
         <v>1</v>
@@ -7528,7 +7607,7 @@
       <c r="F66" s="65"/>
       <c r="G66" s="65"/>
       <c r="H66" s="68" t="str">
-        <f>A66</f>
+        <f t="shared" ref="H66:H70" si="21">A66</f>
         <v xml:space="preserve">BTT Smart Filament Runout Sensor (SFS) </v>
       </c>
       <c r="I66" s="76"/>
@@ -7557,7 +7636,7 @@
     </row>
     <row r="67" spans="1:20">
       <c r="A67" s="103" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B67" s="108">
         <v>2</v>
@@ -7572,11 +7651,11 @@
       <c r="F67" s="113"/>
       <c r="G67" s="113"/>
       <c r="H67" s="114" t="str">
-        <f>A67</f>
+        <f t="shared" si="21"/>
         <v>BTT CB1 Heatsink</v>
       </c>
       <c r="I67" s="107" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J67" s="108">
         <f t="shared" si="18"/>
@@ -7611,15 +7690,15 @@
         <v>392</v>
       </c>
       <c r="S67" s="110" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="T67" s="111" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="68" spans="1:20" ht="30">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" ht="45">
       <c r="A68" s="118" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B68" s="119">
         <v>1</v>
@@ -7634,21 +7713,21 @@
       <c r="F68" s="120"/>
       <c r="G68" s="120"/>
       <c r="H68" s="121" t="str">
-        <f>A68</f>
+        <f t="shared" si="21"/>
         <v>Mandala Roseworks Kinematic center brace for Voron 2.4</v>
       </c>
       <c r="I68" s="122" t="s">
-        <v>483</v>
+        <v>493</v>
       </c>
       <c r="J68" s="119">
-        <f t="shared" ref="J68:J79" si="21">B68</f>
+        <f t="shared" ref="J68:J89" si="22">B68</f>
         <v>1</v>
       </c>
       <c r="K68" s="123">
         <v>35</v>
       </c>
       <c r="L68" s="123">
-        <f t="shared" ref="L68:L79" si="22">J68*K68</f>
+        <f t="shared" ref="L68:L89" si="23">J68*K68</f>
         <v>35</v>
       </c>
       <c r="M68" s="123">
@@ -7658,7 +7737,7 @@
         <v>0</v>
       </c>
       <c r="O68" s="123">
-        <f t="shared" ref="O68:O79" si="23">L68+M68+N68</f>
+        <f t="shared" ref="O68:O89" si="24">L68+M68+N68</f>
         <v>39.06</v>
       </c>
       <c r="P68" s="123">
@@ -7670,15 +7749,15 @@
         <v>280</v>
       </c>
       <c r="S68" s="125" t="s">
-        <v>475</v>
+        <v>495</v>
       </c>
       <c r="T68" s="126" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" ht="45">
       <c r="A69" s="118" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B69" s="119">
         <v>1</v>
@@ -7693,43 +7772,46 @@
       <c r="F69" s="120"/>
       <c r="G69" s="120"/>
       <c r="H69" s="121" t="str">
-        <f>A69</f>
-        <v>Mandala Roseworks Matched height kinematic kit</v>
+        <f t="shared" si="21"/>
+        <v>Mandala Roseworks The "Gripper" E3DV6 Wrench</v>
       </c>
       <c r="I69" s="122" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="J69" s="119">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="K69" s="123">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="L69" s="123">
-        <f t="shared" si="22"/>
-        <v>88</v>
+        <f t="shared" si="23"/>
+        <v>29</v>
       </c>
       <c r="M69" s="123">
-        <v>4.0599999999999996</v>
+        <v>6.27</v>
       </c>
       <c r="N69" s="123">
         <v>0</v>
       </c>
       <c r="O69" s="123">
-        <f t="shared" si="23"/>
-        <v>92.06</v>
+        <f t="shared" si="24"/>
+        <v>35.269999999999996</v>
       </c>
       <c r="P69" s="123">
         <f>O69</f>
-        <v>92.06</v>
-      </c>
-      <c r="Q69" s="122"/>
+        <v>35.269999999999996</v>
+      </c>
+      <c r="Q69" s="124">
+        <f>-1*P69</f>
+        <v>-35.269999999999996</v>
+      </c>
       <c r="R69" s="119" t="s">
         <v>280</v>
       </c>
       <c r="S69" s="125" t="s">
-        <v>477</v>
+        <v>494</v>
       </c>
       <c r="T69" s="126" t="s">
         <v>477</v>
@@ -7737,7 +7819,7 @@
     </row>
     <row r="70" spans="1:20" ht="30">
       <c r="A70" s="118" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B70" s="119">
         <v>1</v>
@@ -7752,54 +7834,54 @@
       <c r="F70" s="120"/>
       <c r="G70" s="120"/>
       <c r="H70" s="121" t="str">
-        <f>A70</f>
-        <v>Mandala Roseworks The "Gripper" E3DV6 Wrench</v>
+        <f t="shared" si="21"/>
+        <v>Layerneer Bed Weld - Original 3D printing adhesive</v>
       </c>
       <c r="I70" s="122" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="J70" s="119">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="J70:J86" si="25">B70</f>
         <v>1</v>
       </c>
       <c r="K70" s="123">
-        <v>29</v>
+        <v>22.95</v>
       </c>
       <c r="L70" s="123">
-        <f t="shared" si="22"/>
-        <v>29</v>
+        <f t="shared" ref="L70:L86" si="26">J70*K70</f>
+        <v>22.95</v>
       </c>
       <c r="M70" s="123">
-        <v>6.27</v>
+        <v>0</v>
       </c>
       <c r="N70" s="123">
         <v>0</v>
       </c>
       <c r="O70" s="123">
-        <f t="shared" si="23"/>
-        <v>35.269999999999996</v>
+        <f t="shared" ref="O70:O86" si="27">L70+M70+N70</f>
+        <v>22.95</v>
       </c>
       <c r="P70" s="123">
         <f>O70</f>
-        <v>35.269999999999996</v>
+        <v>22.95</v>
       </c>
       <c r="Q70" s="124">
         <f>-1*P70</f>
-        <v>-35.269999999999996</v>
+        <v>-22.95</v>
       </c>
       <c r="R70" s="119" t="s">
         <v>280</v>
       </c>
       <c r="S70" s="125" t="s">
+        <v>497</v>
+      </c>
+      <c r="T70" s="126" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" ht="45">
+      <c r="A71" s="118" t="s">
         <v>479</v>
-      </c>
-      <c r="T70" s="126" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" ht="30">
-      <c r="A71" s="118" t="s">
-        <v>480</v>
       </c>
       <c r="B71" s="119">
         <v>1</v>
@@ -7815,204 +7897,356 @@
       <c r="G71" s="120"/>
       <c r="H71" s="121" t="str">
         <f>A71</f>
-        <v>Layerneer Bed Weld - Original 3D printing adhesive</v>
+        <v>Voron Tap - rail w/ optotap v2 (5-24v) and HW kit; from DFH</v>
       </c>
       <c r="I71" s="122" t="s">
-        <v>481</v>
+        <v>492</v>
       </c>
       <c r="J71" s="119">
-        <f t="shared" ref="J71:J76" si="24">B71</f>
+        <f t="shared" ref="J71:J81" si="28">B71</f>
         <v>1</v>
       </c>
       <c r="K71" s="123">
-        <v>22.95</v>
+        <v>45</v>
       </c>
       <c r="L71" s="123">
-        <f t="shared" ref="L71:L76" si="25">J71*K71</f>
-        <v>22.95</v>
+        <f t="shared" ref="L71:L81" si="29">J71*K71</f>
+        <v>45</v>
       </c>
       <c r="M71" s="123">
-        <v>0</v>
+        <f>(20.18/9)*J71</f>
+        <v>2.2422222222222223</v>
       </c>
       <c r="N71" s="123">
         <v>0</v>
       </c>
       <c r="O71" s="123">
-        <f t="shared" ref="O71:O76" si="26">L71+M71+N71</f>
-        <v>22.95</v>
+        <f t="shared" ref="O71:O81" si="30">L71+M71+N71</f>
+        <v>47.242222222222225</v>
       </c>
       <c r="P71" s="123">
-        <f>O71</f>
-        <v>22.95</v>
-      </c>
-      <c r="Q71" s="124">
-        <f>-1*P71</f>
-        <v>-22.95</v>
-      </c>
+        <f>O71-((18.05/9)*J71)</f>
+        <v>45.236666666666672</v>
+      </c>
+      <c r="Q71" s="122"/>
       <c r="R71" s="119" t="s">
         <v>280</v>
       </c>
       <c r="S71" s="125" t="s">
-        <v>485</v>
+        <v>498</v>
       </c>
       <c r="T71" s="126" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="72" spans="1:20">
-      <c r="A72" s="65"/>
-      <c r="B72" s="63"/>
-      <c r="C72" s="63"/>
-      <c r="D72" s="63"/>
-      <c r="E72" s="65"/>
-      <c r="F72" s="65"/>
-      <c r="G72" s="65"/>
-      <c r="H72" s="68"/>
-      <c r="I72" s="76"/>
-      <c r="J72" s="63">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="K72" s="64"/>
-      <c r="L72" s="64">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="M72" s="64"/>
-      <c r="N72" s="64"/>
-      <c r="O72" s="64">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="P72" s="64"/>
-      <c r="Q72" s="76"/>
-      <c r="R72" s="63"/>
-      <c r="S72" s="99"/>
-      <c r="T72" s="100"/>
-    </row>
-    <row r="73" spans="1:20">
-      <c r="A73" s="65"/>
-      <c r="B73" s="63"/>
-      <c r="C73" s="63"/>
-      <c r="D73" s="63"/>
-      <c r="E73" s="65"/>
-      <c r="F73" s="65"/>
-      <c r="G73" s="65"/>
-      <c r="H73" s="68"/>
-      <c r="I73" s="76"/>
-      <c r="J73" s="63">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="K73" s="64"/>
-      <c r="L73" s="64">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="M73" s="64"/>
-      <c r="N73" s="64"/>
-      <c r="O73" s="64">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="P73" s="64"/>
-      <c r="Q73" s="76"/>
-      <c r="R73" s="63"/>
-      <c r="S73" s="99"/>
-      <c r="T73" s="100"/>
-    </row>
-    <row r="74" spans="1:20">
-      <c r="A74" s="65"/>
-      <c r="B74" s="63"/>
-      <c r="C74" s="63"/>
-      <c r="D74" s="63"/>
-      <c r="E74" s="65"/>
-      <c r="F74" s="65"/>
-      <c r="G74" s="65"/>
-      <c r="H74" s="68"/>
-      <c r="I74" s="76"/>
-      <c r="J74" s="63">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="K74" s="64"/>
-      <c r="L74" s="64">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="M74" s="64"/>
-      <c r="N74" s="64"/>
-      <c r="O74" s="64">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="P74" s="64"/>
-      <c r="Q74" s="76"/>
-      <c r="R74" s="63"/>
-      <c r="S74" s="99"/>
-      <c r="T74" s="100"/>
-    </row>
-    <row r="75" spans="1:20">
-      <c r="A75" s="65"/>
-      <c r="B75" s="63"/>
-      <c r="C75" s="63"/>
-      <c r="D75" s="63"/>
-      <c r="E75" s="65"/>
-      <c r="F75" s="65"/>
-      <c r="G75" s="65"/>
-      <c r="H75" s="68"/>
-      <c r="I75" s="76"/>
-      <c r="J75" s="63">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="K75" s="64"/>
-      <c r="L75" s="64">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="M75" s="64"/>
-      <c r="N75" s="64"/>
-      <c r="O75" s="64">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="P75" s="64"/>
-      <c r="Q75" s="76"/>
-      <c r="R75" s="63"/>
-      <c r="S75" s="99"/>
-      <c r="T75" s="100"/>
-    </row>
-    <row r="76" spans="1:20">
-      <c r="A76" s="65"/>
-      <c r="B76" s="63"/>
-      <c r="C76" s="63"/>
-      <c r="D76" s="63"/>
-      <c r="E76" s="65"/>
-      <c r="F76" s="65"/>
-      <c r="G76" s="65"/>
-      <c r="H76" s="68"/>
-      <c r="I76" s="76"/>
-      <c r="J76" s="63">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="K76" s="64"/>
-      <c r="L76" s="64">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="M76" s="64"/>
-      <c r="N76" s="64"/>
-      <c r="O76" s="64">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="P76" s="64"/>
-      <c r="Q76" s="76"/>
-      <c r="R76" s="63"/>
-      <c r="S76" s="99"/>
-      <c r="T76" s="100"/>
+    <row r="72" spans="1:20" ht="30">
+      <c r="A72" s="118" t="s">
+        <v>481</v>
+      </c>
+      <c r="B72" s="119">
+        <v>2</v>
+      </c>
+      <c r="C72" s="119" t="s">
+        <v>313</v>
+      </c>
+      <c r="D72" s="119" t="s">
+        <v>298</v>
+      </c>
+      <c r="E72" s="120"/>
+      <c r="F72" s="120"/>
+      <c r="G72" s="120"/>
+      <c r="H72" s="121" t="str">
+        <f>A72</f>
+        <v>Nightlight on a stick - LED Strip; from DFH</v>
+      </c>
+      <c r="I72" s="122" t="s">
+        <v>486</v>
+      </c>
+      <c r="J72" s="119">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="K72" s="123">
+        <v>17.5</v>
+      </c>
+      <c r="L72" s="123">
+        <f t="shared" si="29"/>
+        <v>35</v>
+      </c>
+      <c r="M72" s="123">
+        <f t="shared" ref="M72:M76" si="31">(20.18/9)*J72</f>
+        <v>4.4844444444444447</v>
+      </c>
+      <c r="N72" s="123">
+        <v>0</v>
+      </c>
+      <c r="O72" s="123">
+        <f t="shared" si="30"/>
+        <v>39.484444444444442</v>
+      </c>
+      <c r="P72" s="123">
+        <f t="shared" ref="P72:P76" si="32">O72-((18.05/9)*J72)</f>
+        <v>35.473333333333329</v>
+      </c>
+      <c r="Q72" s="124">
+        <f>-1*P72</f>
+        <v>-35.473333333333329</v>
+      </c>
+      <c r="R72" s="119" t="s">
+        <v>280</v>
+      </c>
+      <c r="S72" s="125" t="s">
+        <v>488</v>
+      </c>
+      <c r="T72" s="126" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" ht="30">
+      <c r="A73" s="118" t="s">
+        <v>482</v>
+      </c>
+      <c r="B73" s="119">
+        <v>2</v>
+      </c>
+      <c r="C73" s="119" t="s">
+        <v>313</v>
+      </c>
+      <c r="D73" s="119" t="s">
+        <v>298</v>
+      </c>
+      <c r="E73" s="120"/>
+      <c r="F73" s="120"/>
+      <c r="G73" s="120"/>
+      <c r="H73" s="121" t="str">
+        <f>A73</f>
+        <v>Disco stick on black PCB - LED Strip; from DFH</v>
+      </c>
+      <c r="I73" s="122" t="s">
+        <v>486</v>
+      </c>
+      <c r="J73" s="119">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="K73" s="123">
+        <v>16.5</v>
+      </c>
+      <c r="L73" s="123">
+        <f t="shared" si="29"/>
+        <v>33</v>
+      </c>
+      <c r="M73" s="123">
+        <f t="shared" si="31"/>
+        <v>4.4844444444444447</v>
+      </c>
+      <c r="N73" s="123">
+        <v>0</v>
+      </c>
+      <c r="O73" s="123">
+        <f t="shared" si="30"/>
+        <v>37.484444444444442</v>
+      </c>
+      <c r="P73" s="123">
+        <f t="shared" si="32"/>
+        <v>33.473333333333329</v>
+      </c>
+      <c r="Q73" s="122"/>
+      <c r="R73" s="119" t="s">
+        <v>280</v>
+      </c>
+      <c r="S73" s="125" t="s">
+        <v>488</v>
+      </c>
+      <c r="T73" s="126" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" ht="30">
+      <c r="A74" s="118" t="s">
+        <v>484</v>
+      </c>
+      <c r="B74" s="119">
+        <v>1</v>
+      </c>
+      <c r="C74" s="119" t="s">
+        <v>313</v>
+      </c>
+      <c r="D74" s="119" t="s">
+        <v>298</v>
+      </c>
+      <c r="E74" s="120"/>
+      <c r="F74" s="120"/>
+      <c r="G74" s="120"/>
+      <c r="H74" s="121" t="str">
+        <f>A74</f>
+        <v>OV5640 Camera Module; from DFH</v>
+      </c>
+      <c r="I74" s="122" t="s">
+        <v>486</v>
+      </c>
+      <c r="J74" s="119">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="K74" s="123">
+        <v>32.5</v>
+      </c>
+      <c r="L74" s="123">
+        <f t="shared" si="29"/>
+        <v>32.5</v>
+      </c>
+      <c r="M74" s="123">
+        <f t="shared" si="31"/>
+        <v>2.2422222222222223</v>
+      </c>
+      <c r="N74" s="123">
+        <v>0</v>
+      </c>
+      <c r="O74" s="123">
+        <f t="shared" si="30"/>
+        <v>34.742222222222225</v>
+      </c>
+      <c r="P74" s="123">
+        <f t="shared" si="32"/>
+        <v>32.736666666666672</v>
+      </c>
+      <c r="Q74" s="122"/>
+      <c r="R74" s="119" t="s">
+        <v>280</v>
+      </c>
+      <c r="S74" s="125" t="s">
+        <v>488</v>
+      </c>
+      <c r="T74" s="126" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" ht="30">
+      <c r="A75" s="118" t="s">
+        <v>485</v>
+      </c>
+      <c r="B75" s="119">
+        <v>2</v>
+      </c>
+      <c r="C75" s="119" t="s">
+        <v>313</v>
+      </c>
+      <c r="D75" s="119" t="s">
+        <v>383</v>
+      </c>
+      <c r="E75" s="120"/>
+      <c r="F75" s="120"/>
+      <c r="G75" s="120"/>
+      <c r="H75" s="121" t="str">
+        <f>A75</f>
+        <v>Seeeduino XIAO; from DFH</v>
+      </c>
+      <c r="I75" s="122" t="s">
+        <v>490</v>
+      </c>
+      <c r="J75" s="119">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="K75" s="123">
+        <v>10</v>
+      </c>
+      <c r="L75" s="123">
+        <f t="shared" si="29"/>
+        <v>20</v>
+      </c>
+      <c r="M75" s="123">
+        <f t="shared" si="31"/>
+        <v>4.4844444444444447</v>
+      </c>
+      <c r="N75" s="123">
+        <v>0</v>
+      </c>
+      <c r="O75" s="123">
+        <f t="shared" si="30"/>
+        <v>24.484444444444446</v>
+      </c>
+      <c r="P75" s="123">
+        <f t="shared" si="32"/>
+        <v>20.473333333333336</v>
+      </c>
+      <c r="Q75" s="124">
+        <f>-1*(P75/2)</f>
+        <v>-10.236666666666668</v>
+      </c>
+      <c r="R75" s="119" t="s">
+        <v>280</v>
+      </c>
+      <c r="S75" s="125" t="s">
+        <v>488</v>
+      </c>
+      <c r="T75" s="126" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" ht="30">
+      <c r="A76" s="118" t="s">
+        <v>483</v>
+      </c>
+      <c r="B76" s="119">
+        <v>1</v>
+      </c>
+      <c r="C76" s="119" t="s">
+        <v>313</v>
+      </c>
+      <c r="D76" s="119" t="s">
+        <v>383</v>
+      </c>
+      <c r="E76" s="120"/>
+      <c r="F76" s="120"/>
+      <c r="G76" s="120"/>
+      <c r="H76" s="121" t="str">
+        <f>A76</f>
+        <v>Daylight on a stick on black PCB; from DFH</v>
+      </c>
+      <c r="I76" s="122" t="s">
+        <v>489</v>
+      </c>
+      <c r="J76" s="119">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="K76" s="123">
+        <v>15</v>
+      </c>
+      <c r="L76" s="123">
+        <f t="shared" si="29"/>
+        <v>15</v>
+      </c>
+      <c r="M76" s="123">
+        <f t="shared" si="31"/>
+        <v>2.2422222222222223</v>
+      </c>
+      <c r="N76" s="123">
+        <v>0</v>
+      </c>
+      <c r="O76" s="123">
+        <f t="shared" si="30"/>
+        <v>17.242222222222221</v>
+      </c>
+      <c r="P76" s="123">
+        <f t="shared" si="32"/>
+        <v>15.236666666666665</v>
+      </c>
+      <c r="Q76" s="124">
+        <f>-1*P76</f>
+        <v>-15.236666666666665</v>
+      </c>
+      <c r="R76" s="119" t="s">
+        <v>280</v>
+      </c>
+      <c r="S76" s="125" t="s">
+        <v>488</v>
+      </c>
+      <c r="T76" s="126" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="77" spans="1:20">
       <c r="A77" s="65"/>
@@ -8025,18 +8259,18 @@
       <c r="H77" s="68"/>
       <c r="I77" s="76"/>
       <c r="J77" s="63">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K77" s="64"/>
       <c r="L77" s="64">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="M77" s="64"/>
       <c r="N77" s="64"/>
       <c r="O77" s="64">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="P77" s="64"/>
@@ -8056,18 +8290,18 @@
       <c r="H78" s="68"/>
       <c r="I78" s="76"/>
       <c r="J78" s="63">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K78" s="64"/>
       <c r="L78" s="64">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="M78" s="64"/>
       <c r="N78" s="64"/>
       <c r="O78" s="64">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="P78" s="64"/>
@@ -8087,18 +8321,18 @@
       <c r="H79" s="68"/>
       <c r="I79" s="76"/>
       <c r="J79" s="63">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K79" s="64"/>
       <c r="L79" s="64">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="M79" s="64"/>
       <c r="N79" s="64"/>
       <c r="O79" s="64">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="P79" s="64"/>
@@ -8118,18 +8352,18 @@
       <c r="H80" s="68"/>
       <c r="I80" s="76"/>
       <c r="J80" s="63">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K80" s="64"/>
       <c r="L80" s="64">
-        <f t="shared" si="16"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="M80" s="64"/>
       <c r="N80" s="64"/>
       <c r="O80" s="64">
-        <f t="shared" si="20"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="P80" s="64"/>
@@ -8149,18 +8383,18 @@
       <c r="H81" s="68"/>
       <c r="I81" s="76"/>
       <c r="J81" s="63">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K81" s="64"/>
       <c r="L81" s="64">
-        <f t="shared" si="16"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="M81" s="64"/>
       <c r="N81" s="64"/>
       <c r="O81" s="64">
-        <f t="shared" si="20"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="P81" s="64"/>
@@ -8180,18 +8414,18 @@
       <c r="H82" s="68"/>
       <c r="I82" s="76"/>
       <c r="J82" s="63">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K82" s="64"/>
       <c r="L82" s="64">
-        <f t="shared" si="16"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="M82" s="64"/>
       <c r="N82" s="64"/>
       <c r="O82" s="64">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P82" s="64"/>
@@ -8200,7 +8434,7 @@
       <c r="S82" s="99"/>
       <c r="T82" s="100"/>
     </row>
-    <row r="83" spans="1:20" ht="17" thickBot="1">
+    <row r="83" spans="1:20">
       <c r="A83" s="65"/>
       <c r="B83" s="63"/>
       <c r="C83" s="63"/>
@@ -8210,47 +8444,57 @@
       <c r="G83" s="65"/>
       <c r="H83" s="68"/>
       <c r="I83" s="76"/>
-      <c r="J83" s="63"/>
+      <c r="J83" s="63">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
       <c r="K83" s="64"/>
-      <c r="L83" s="64"/>
+      <c r="L83" s="64">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
       <c r="M83" s="64"/>
       <c r="N83" s="64"/>
-      <c r="O83" s="64"/>
+      <c r="O83" s="64">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
       <c r="P83" s="64"/>
-      <c r="Q83" s="62"/>
-      <c r="S83" s="65"/>
-      <c r="T83" s="65"/>
-    </row>
-    <row r="84" spans="1:20" ht="18" thickTop="1">
+      <c r="Q83" s="76"/>
+      <c r="R83" s="63"/>
+      <c r="S83" s="99"/>
+      <c r="T83" s="100"/>
+    </row>
+    <row r="84" spans="1:20">
       <c r="A84" s="65"/>
       <c r="B84" s="63"/>
       <c r="C84" s="63"/>
       <c r="D84" s="63"/>
       <c r="E84" s="65"/>
       <c r="F84" s="65"/>
-      <c r="G84" s="82"/>
-      <c r="H84" s="78"/>
-      <c r="I84" s="146" t="s">
-        <v>426</v>
-      </c>
-      <c r="J84" s="79"/>
-      <c r="K84" s="78"/>
-      <c r="L84" s="78"/>
-      <c r="M84" s="78"/>
-      <c r="N84" s="78"/>
-      <c r="O84" s="78">
-        <f>SUM(O3:O82)</f>
-        <v>2594.6099999999992</v>
-      </c>
-      <c r="P84" s="78">
-        <f>SUM(P3:P82)</f>
-        <v>1619.44</v>
-      </c>
-      <c r="Q84" s="78">
-        <f>SUM(Q3:Q82)</f>
-        <v>-130.17999999999998</v>
-      </c>
-      <c r="R84" s="83"/>
+      <c r="G84" s="65"/>
+      <c r="H84" s="68"/>
+      <c r="I84" s="76"/>
+      <c r="J84" s="63">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="K84" s="64"/>
+      <c r="L84" s="64">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="M84" s="64"/>
+      <c r="N84" s="64"/>
+      <c r="O84" s="64">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="P84" s="64"/>
+      <c r="Q84" s="76"/>
+      <c r="R84" s="63"/>
+      <c r="S84" s="99"/>
+      <c r="T84" s="100"/>
     </row>
     <row r="85" spans="1:20">
       <c r="A85" s="65"/>
@@ -8262,20 +8506,26 @@
       <c r="G85" s="65"/>
       <c r="H85" s="68"/>
       <c r="I85" s="76"/>
-      <c r="J85" s="63"/>
+      <c r="J85" s="63">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
       <c r="K85" s="64"/>
-      <c r="L85" s="64"/>
+      <c r="L85" s="64">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
       <c r="M85" s="64"/>
       <c r="N85" s="64"/>
-      <c r="O85" s="64"/>
+      <c r="O85" s="64">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
       <c r="P85" s="64"/>
-      <c r="Q85" s="65" t="s">
-        <v>433</v>
-      </c>
-      <c r="R85" s="64">
-        <f>O84-P84+Q84</f>
-        <v>844.98999999999921</v>
-      </c>
+      <c r="Q85" s="76"/>
+      <c r="R85" s="63"/>
+      <c r="S85" s="99"/>
+      <c r="T85" s="100"/>
     </row>
     <row r="86" spans="1:20">
       <c r="A86" s="65"/>
@@ -8287,20 +8537,26 @@
       <c r="G86" s="65"/>
       <c r="H86" s="68"/>
       <c r="I86" s="76"/>
-      <c r="J86" s="63"/>
+      <c r="J86" s="63">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
       <c r="K86" s="64"/>
-      <c r="L86" s="64"/>
+      <c r="L86" s="64">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
       <c r="M86" s="64"/>
       <c r="N86" s="64"/>
-      <c r="O86" s="64"/>
+      <c r="O86" s="64">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
       <c r="P86" s="64"/>
-      <c r="Q86" s="65" t="s">
-        <v>430</v>
-      </c>
-      <c r="R86" s="64">
-        <f>P84</f>
-        <v>1619.44</v>
-      </c>
+      <c r="Q86" s="76"/>
+      <c r="R86" s="63"/>
+      <c r="S86" s="99"/>
+      <c r="T86" s="100"/>
     </row>
     <row r="87" spans="1:20">
       <c r="A87" s="65"/>
@@ -8312,20 +8568,26 @@
       <c r="G87" s="65"/>
       <c r="H87" s="68"/>
       <c r="I87" s="76"/>
-      <c r="J87" s="63"/>
+      <c r="J87" s="63">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
       <c r="K87" s="64"/>
-      <c r="L87" s="64"/>
+      <c r="L87" s="64">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
       <c r="M87" s="64"/>
       <c r="N87" s="64"/>
-      <c r="O87" s="64"/>
+      <c r="O87" s="64">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
       <c r="P87" s="64"/>
-      <c r="Q87" s="65" t="s">
-        <v>431</v>
-      </c>
-      <c r="R87" s="64">
-        <f>SUM(Q3:Q82)*-1</f>
-        <v>130.17999999999998</v>
-      </c>
+      <c r="Q87" s="76"/>
+      <c r="R87" s="63"/>
+      <c r="S87" s="99"/>
+      <c r="T87" s="100"/>
     </row>
     <row r="88" spans="1:20">
       <c r="A88" s="65"/>
@@ -8336,20 +8598,27 @@
       <c r="F88" s="65"/>
       <c r="G88" s="65"/>
       <c r="H88" s="68"/>
-      <c r="I88" s="62"/>
-      <c r="J88" s="63"/>
+      <c r="I88" s="76"/>
+      <c r="J88" s="63">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
       <c r="K88" s="64"/>
-      <c r="L88" s="64"/>
+      <c r="L88" s="64">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
       <c r="M88" s="64"/>
       <c r="N88" s="64"/>
-      <c r="O88" s="64"/>
+      <c r="O88" s="64">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
       <c r="P88" s="64"/>
-      <c r="Q88" s="89" t="s">
-        <v>447</v>
-      </c>
-      <c r="R88" s="90">
-        <v>146.82</v>
-      </c>
+      <c r="Q88" s="76"/>
+      <c r="R88" s="63"/>
+      <c r="S88" s="99"/>
+      <c r="T88" s="100"/>
     </row>
     <row r="89" spans="1:20">
       <c r="A89" s="65"/>
@@ -8360,20 +8629,27 @@
       <c r="F89" s="65"/>
       <c r="G89" s="65"/>
       <c r="H89" s="68"/>
-      <c r="I89" s="62"/>
-      <c r="J89" s="63"/>
+      <c r="I89" s="76"/>
+      <c r="J89" s="63">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
       <c r="K89" s="64"/>
-      <c r="L89" s="64"/>
+      <c r="L89" s="64">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
       <c r="M89" s="64"/>
       <c r="N89" s="64"/>
-      <c r="O89" s="64"/>
+      <c r="O89" s="64">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
       <c r="P89" s="64"/>
-      <c r="Q89" s="89" t="s">
-        <v>448</v>
-      </c>
-      <c r="R89" s="90">
-        <v>71.98</v>
-      </c>
+      <c r="Q89" s="76"/>
+      <c r="R89" s="63"/>
+      <c r="S89" s="99"/>
+      <c r="T89" s="100"/>
     </row>
     <row r="90" spans="1:20">
       <c r="A90" s="65"/>
@@ -8384,21 +8660,27 @@
       <c r="F90" s="65"/>
       <c r="G90" s="65"/>
       <c r="H90" s="68"/>
-      <c r="I90" s="62"/>
-      <c r="J90" s="63"/>
+      <c r="I90" s="76"/>
+      <c r="J90" s="63">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
       <c r="K90" s="64"/>
-      <c r="L90" s="64"/>
+      <c r="L90" s="64">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
       <c r="M90" s="64"/>
       <c r="N90" s="64"/>
-      <c r="O90" s="64"/>
+      <c r="O90" s="64">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
       <c r="P90" s="64"/>
-      <c r="Q90" s="65" t="s">
-        <v>449</v>
-      </c>
-      <c r="R90" s="64">
-        <f>530.9+136.98+543.42+131.12+35.27+22.95</f>
-        <v>1400.64</v>
-      </c>
+      <c r="Q90" s="76"/>
+      <c r="R90" s="63"/>
+      <c r="S90" s="99"/>
+      <c r="T90" s="100"/>
     </row>
     <row r="91" spans="1:20">
       <c r="A91" s="65"/>
@@ -8409,65 +8691,336 @@
       <c r="F91" s="65"/>
       <c r="G91" s="65"/>
       <c r="H91" s="68"/>
-      <c r="I91" s="62"/>
-      <c r="J91" s="63"/>
+      <c r="I91" s="76"/>
+      <c r="J91" s="63">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
       <c r="K91" s="64"/>
-      <c r="L91" s="64"/>
+      <c r="L91" s="64">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
       <c r="M91" s="64"/>
       <c r="N91" s="64"/>
-      <c r="O91" s="64"/>
+      <c r="O91" s="64">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
       <c r="P91" s="64"/>
-      <c r="Q91" s="65"/>
-      <c r="R91" s="64"/>
+      <c r="Q91" s="76"/>
+      <c r="R91" s="63"/>
+      <c r="S91" s="99"/>
+      <c r="T91" s="100"/>
     </row>
     <row r="92" spans="1:20">
+      <c r="A92" s="65"/>
+      <c r="B92" s="63"/>
+      <c r="C92" s="63"/>
+      <c r="D92" s="63"/>
+      <c r="E92" s="65"/>
+      <c r="F92" s="65"/>
+      <c r="G92" s="65"/>
       <c r="H92" s="68"/>
-      <c r="Q92" s="57"/>
-      <c r="R92" s="64"/>
-    </row>
-    <row r="93" spans="1:20">
+      <c r="I92" s="76"/>
+      <c r="J92" s="63">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K92" s="64"/>
+      <c r="L92" s="64">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="M92" s="64"/>
+      <c r="N92" s="64"/>
+      <c r="O92" s="64">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="P92" s="64"/>
+      <c r="Q92" s="76"/>
+      <c r="R92" s="63"/>
+      <c r="S92" s="99"/>
+      <c r="T92" s="100"/>
+    </row>
+    <row r="93" spans="1:20" ht="17" thickBot="1">
+      <c r="A93" s="65"/>
+      <c r="B93" s="63"/>
+      <c r="C93" s="63"/>
+      <c r="D93" s="63"/>
+      <c r="E93" s="65"/>
+      <c r="F93" s="65"/>
+      <c r="G93" s="65"/>
       <c r="H93" s="68"/>
-      <c r="Q93" s="57"/>
-      <c r="R93" s="64"/>
-    </row>
-    <row r="94" spans="1:20">
-      <c r="H94" s="68"/>
-      <c r="Q94" s="57"/>
-      <c r="R94" s="64"/>
+      <c r="I93" s="76"/>
+      <c r="J93" s="63"/>
+      <c r="K93" s="64"/>
+      <c r="L93" s="64"/>
+      <c r="M93" s="64"/>
+      <c r="N93" s="64"/>
+      <c r="O93" s="64"/>
+      <c r="P93" s="64"/>
+      <c r="Q93" s="62"/>
+      <c r="S93" s="65"/>
+      <c r="T93" s="65"/>
+    </row>
+    <row r="94" spans="1:20" ht="18" thickTop="1">
+      <c r="A94" s="65"/>
+      <c r="B94" s="63"/>
+      <c r="C94" s="63"/>
+      <c r="D94" s="63"/>
+      <c r="E94" s="65"/>
+      <c r="F94" s="65"/>
+      <c r="G94" s="82"/>
+      <c r="H94" s="78"/>
+      <c r="I94" s="132" t="s">
+        <v>426</v>
+      </c>
+      <c r="J94" s="79"/>
+      <c r="K94" s="78"/>
+      <c r="L94" s="78">
+        <f t="shared" ref="L94:N94" si="33">SUM(L3:L92)</f>
+        <v>2598.9099999999994</v>
+      </c>
+      <c r="M94" s="78">
+        <f t="shared" si="33"/>
+        <v>111.39000000000001</v>
+      </c>
+      <c r="N94" s="78">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="O94" s="78">
+        <f>SUM(O3:O92)</f>
+        <v>2710.2999999999988</v>
+      </c>
+      <c r="P94" s="78">
+        <f>SUM(P3:P92)</f>
+        <v>1802.0700000000002</v>
+      </c>
+      <c r="Q94" s="78">
+        <f>SUM(Q3:Q92)</f>
+        <v>-191.12666666666667</v>
+      </c>
+      <c r="R94" s="83"/>
     </row>
     <row r="95" spans="1:20">
-      <c r="Q95" s="57"/>
-      <c r="R95" s="64"/>
+      <c r="A95" s="65"/>
+      <c r="B95" s="63"/>
+      <c r="C95" s="63"/>
+      <c r="D95" s="63"/>
+      <c r="E95" s="65"/>
+      <c r="F95" s="65"/>
+      <c r="G95" s="65"/>
+      <c r="H95" s="68"/>
+      <c r="I95" s="76"/>
+      <c r="J95" s="63"/>
+      <c r="K95" s="64"/>
+      <c r="L95" s="64"/>
+      <c r="M95" s="64"/>
+      <c r="N95" s="64"/>
+      <c r="O95" s="64"/>
+      <c r="P95" s="64"/>
+      <c r="Q95" s="65" t="s">
+        <v>433</v>
+      </c>
+      <c r="R95" s="64">
+        <f>O94-P94+Q94</f>
+        <v>717.10333333333199</v>
+      </c>
     </row>
     <row r="96" spans="1:20">
-      <c r="Q96" s="57"/>
-      <c r="R96" s="64"/>
-    </row>
-    <row r="97" spans="17:18">
-      <c r="Q97" s="57"/>
-      <c r="R97" s="64"/>
-    </row>
-    <row r="98" spans="17:18">
-      <c r="Q98" s="57"/>
-      <c r="R98" s="64"/>
-    </row>
-    <row r="99" spans="17:18">
-      <c r="Q99" s="57"/>
-      <c r="R99" s="64"/>
-    </row>
-    <row r="100" spans="17:18">
-      <c r="Q100" s="57"/>
-      <c r="R100" s="64"/>
-    </row>
-    <row r="101" spans="17:18">
+      <c r="A96" s="65"/>
+      <c r="B96" s="63"/>
+      <c r="C96" s="63"/>
+      <c r="D96" s="63"/>
+      <c r="E96" s="65"/>
+      <c r="F96" s="65"/>
+      <c r="G96" s="65"/>
+      <c r="H96" s="68"/>
+      <c r="I96" s="76"/>
+      <c r="J96" s="63"/>
+      <c r="K96" s="64"/>
+      <c r="L96" s="64"/>
+      <c r="M96" s="64"/>
+      <c r="N96" s="64"/>
+      <c r="O96" s="64"/>
+      <c r="P96" s="64"/>
+      <c r="Q96" s="65" t="s">
+        <v>430</v>
+      </c>
+      <c r="R96" s="64">
+        <f>P94</f>
+        <v>1802.0700000000002</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18">
+      <c r="A97" s="65"/>
+      <c r="B97" s="63"/>
+      <c r="C97" s="63"/>
+      <c r="D97" s="63"/>
+      <c r="E97" s="65"/>
+      <c r="F97" s="65"/>
+      <c r="G97" s="65"/>
+      <c r="H97" s="68"/>
+      <c r="I97" s="76"/>
+      <c r="J97" s="63"/>
+      <c r="K97" s="64"/>
+      <c r="L97" s="64"/>
+      <c r="M97" s="64"/>
+      <c r="N97" s="64"/>
+      <c r="O97" s="64"/>
+      <c r="P97" s="64"/>
+      <c r="Q97" s="65" t="s">
+        <v>431</v>
+      </c>
+      <c r="R97" s="64">
+        <f>SUM(Q3:Q92)*-1</f>
+        <v>191.12666666666667</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18">
+      <c r="A98" s="65"/>
+      <c r="B98" s="63"/>
+      <c r="C98" s="63"/>
+      <c r="D98" s="63"/>
+      <c r="E98" s="65"/>
+      <c r="F98" s="65"/>
+      <c r="G98" s="65"/>
+      <c r="H98" s="68"/>
+      <c r="I98" s="62"/>
+      <c r="J98" s="63"/>
+      <c r="K98" s="64"/>
+      <c r="L98" s="64"/>
+      <c r="M98" s="64"/>
+      <c r="N98" s="64"/>
+      <c r="O98" s="64"/>
+      <c r="P98" s="64"/>
+      <c r="Q98" s="89" t="s">
+        <v>446</v>
+      </c>
+      <c r="R98" s="90">
+        <v>146.82</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18">
+      <c r="A99" s="65"/>
+      <c r="B99" s="63"/>
+      <c r="C99" s="63"/>
+      <c r="D99" s="63"/>
+      <c r="E99" s="65"/>
+      <c r="F99" s="65"/>
+      <c r="G99" s="65"/>
+      <c r="H99" s="68"/>
+      <c r="I99" s="62"/>
+      <c r="J99" s="63"/>
+      <c r="K99" s="64"/>
+      <c r="L99" s="64"/>
+      <c r="M99" s="64"/>
+      <c r="N99" s="64"/>
+      <c r="O99" s="64"/>
+      <c r="P99" s="64"/>
+      <c r="Q99" s="89" t="s">
+        <v>447</v>
+      </c>
+      <c r="R99" s="90">
+        <v>71.98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18">
+      <c r="A100" s="65"/>
+      <c r="B100" s="63"/>
+      <c r="C100" s="63"/>
+      <c r="D100" s="63"/>
+      <c r="E100" s="65"/>
+      <c r="F100" s="65"/>
+      <c r="G100" s="65"/>
+      <c r="H100" s="68"/>
+      <c r="I100" s="62"/>
+      <c r="J100" s="63"/>
+      <c r="K100" s="64"/>
+      <c r="L100" s="64"/>
+      <c r="M100" s="64"/>
+      <c r="N100" s="64"/>
+      <c r="O100" s="64"/>
+      <c r="P100" s="64"/>
+      <c r="Q100" s="65" t="s">
+        <v>448</v>
+      </c>
+      <c r="R100" s="64">
+        <f>530.9+136.98+543.42+131.12+35.27+22.95+182.63</f>
+        <v>1583.27</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18">
+      <c r="A101" s="65"/>
+      <c r="B101" s="63"/>
+      <c r="C101" s="63"/>
+      <c r="D101" s="63"/>
+      <c r="E101" s="65"/>
+      <c r="F101" s="65"/>
+      <c r="G101" s="65"/>
+      <c r="H101" s="68"/>
+      <c r="I101" s="62"/>
+      <c r="J101" s="63"/>
+      <c r="K101" s="64"/>
+      <c r="L101" s="64"/>
+      <c r="M101" s="64"/>
+      <c r="N101" s="64"/>
+      <c r="O101" s="64"/>
+      <c r="P101" s="64"/>
+      <c r="Q101" s="65"/>
       <c r="R101" s="64"/>
+    </row>
+    <row r="102" spans="1:18">
+      <c r="H102" s="68"/>
+      <c r="Q102" s="57"/>
+      <c r="R102" s="64"/>
+    </row>
+    <row r="103" spans="1:18">
+      <c r="H103" s="68"/>
+      <c r="Q103" s="57"/>
+      <c r="R103" s="64"/>
+    </row>
+    <row r="104" spans="1:18">
+      <c r="H104" s="68"/>
+      <c r="Q104" s="57"/>
+      <c r="R104" s="64"/>
+    </row>
+    <row r="105" spans="1:18">
+      <c r="Q105" s="57"/>
+      <c r="R105" s="64"/>
+    </row>
+    <row r="106" spans="1:18">
+      <c r="Q106" s="57"/>
+      <c r="R106" s="64"/>
+    </row>
+    <row r="107" spans="1:18">
+      <c r="Q107" s="57"/>
+      <c r="R107" s="64"/>
+    </row>
+    <row r="108" spans="1:18">
+      <c r="Q108" s="57"/>
+      <c r="R108" s="64"/>
+    </row>
+    <row r="109" spans="1:18">
+      <c r="Q109" s="57"/>
+      <c r="R109" s="64"/>
+    </row>
+    <row r="110" spans="1:18">
+      <c r="Q110" s="57"/>
+      <c r="R110" s="64"/>
+    </row>
+    <row r="111" spans="1:18">
+      <c r="R111" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:T1"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R82" xr:uid="{DB0DC2B0-407F-9946-A6F5-0517B7729D5C}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R92" xr:uid="{DB0DC2B0-407F-9946-A6F5-0517B7729D5C}">
       <formula1>$AD$4:$AD$10</formula1>
     </dataValidation>
   </dataValidations>
@@ -8565,12 +9118,18 @@
     <hyperlink ref="F39" r:id="rId91" xr:uid="{88603DA9-A020-654B-AB72-175FC13D034C}"/>
     <hyperlink ref="A47" r:id="rId92" xr:uid="{D2A36D58-E15F-7E44-8EA3-6C4685C8E3B6}"/>
     <hyperlink ref="A68" r:id="rId93" xr:uid="{85B2FF62-2608-CB48-BB1D-A10E8DC456BE}"/>
-    <hyperlink ref="A69" r:id="rId94" xr:uid="{9C431DE7-49E1-604B-B724-7A37503178F1}"/>
-    <hyperlink ref="A70" r:id="rId95" xr:uid="{74A5D6C7-F7CE-964A-91E1-00B79BAFEB5B}"/>
-    <hyperlink ref="A71" r:id="rId96" xr:uid="{D4E64753-7DF1-BC46-9783-EE4EA90305B4}"/>
+    <hyperlink ref="A69" r:id="rId94" xr:uid="{74A5D6C7-F7CE-964A-91E1-00B79BAFEB5B}"/>
+    <hyperlink ref="A70" r:id="rId95" xr:uid="{D4E64753-7DF1-BC46-9783-EE4EA90305B4}"/>
+    <hyperlink ref="E61" r:id="rId96" xr:uid="{A782B948-F32A-DF45-85B9-9862EE145443}"/>
+    <hyperlink ref="A71" r:id="rId97" xr:uid="{E39F14A3-4AE1-FE41-AADE-2275E109D5E7}"/>
+    <hyperlink ref="A72" r:id="rId98" xr:uid="{B31ACB39-14B2-F342-BF62-356704801E5C}"/>
+    <hyperlink ref="A73" r:id="rId99" xr:uid="{E0DFEB3E-1B65-104C-895C-63E7833C538C}"/>
+    <hyperlink ref="A74" r:id="rId100" xr:uid="{D4CC3802-04BE-B14C-8DCE-3AB15733D983}"/>
+    <hyperlink ref="A75" r:id="rId101" xr:uid="{86DAA688-EE23-6A4A-A517-12DB5FD32832}"/>
+    <hyperlink ref="A76" r:id="rId102" xr:uid="{A6FC9FB5-F7AB-7E42-9201-841F5EB0F339}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId97"/>
+  <legacyDrawing r:id="rId103"/>
 </worksheet>
 </file>
 
@@ -10548,24 +11107,24 @@
       </c>
     </row>
     <row r="73" spans="1:16" ht="17" thickBot="1">
-      <c r="A73" s="133" t="s">
+      <c r="A73" s="134" t="s">
         <v>288</v>
       </c>
-      <c r="B73" s="134"/>
-      <c r="C73" s="134"/>
-      <c r="D73" s="134"/>
-      <c r="E73" s="134"/>
-      <c r="F73" s="134"/>
-      <c r="G73" s="134"/>
-      <c r="H73" s="134"/>
-      <c r="I73" s="134"/>
-      <c r="J73" s="134"/>
-      <c r="K73" s="134"/>
-      <c r="L73" s="134"/>
-      <c r="M73" s="134"/>
-      <c r="N73" s="134"/>
-      <c r="O73" s="134"/>
-      <c r="P73" s="135"/>
+      <c r="B73" s="135"/>
+      <c r="C73" s="135"/>
+      <c r="D73" s="135"/>
+      <c r="E73" s="135"/>
+      <c r="F73" s="135"/>
+      <c r="G73" s="135"/>
+      <c r="H73" s="135"/>
+      <c r="I73" s="135"/>
+      <c r="J73" s="135"/>
+      <c r="K73" s="135"/>
+      <c r="L73" s="135"/>
+      <c r="M73" s="135"/>
+      <c r="N73" s="135"/>
+      <c r="O73" s="135"/>
+      <c r="P73" s="136"/>
     </row>
     <row r="74" spans="1:16" ht="17">
       <c r="A74" s="13" t="s">
@@ -10773,24 +11332,24 @@
     </row>
     <row r="85" spans="1:16" ht="17" thickBot="1"/>
     <row r="86" spans="1:16" ht="17" thickBot="1">
-      <c r="A86" s="136" t="s">
+      <c r="A86" s="137" t="s">
         <v>208</v>
       </c>
-      <c r="B86" s="137"/>
-      <c r="C86" s="137"/>
-      <c r="D86" s="137"/>
-      <c r="E86" s="137"/>
-      <c r="F86" s="137"/>
-      <c r="G86" s="137"/>
-      <c r="H86" s="137"/>
-      <c r="I86" s="137"/>
-      <c r="J86" s="137"/>
-      <c r="K86" s="137"/>
-      <c r="L86" s="137"/>
-      <c r="M86" s="137"/>
-      <c r="N86" s="137"/>
-      <c r="O86" s="137"/>
-      <c r="P86" s="138"/>
+      <c r="B86" s="138"/>
+      <c r="C86" s="138"/>
+      <c r="D86" s="138"/>
+      <c r="E86" s="138"/>
+      <c r="F86" s="138"/>
+      <c r="G86" s="138"/>
+      <c r="H86" s="138"/>
+      <c r="I86" s="138"/>
+      <c r="J86" s="138"/>
+      <c r="K86" s="138"/>
+      <c r="L86" s="138"/>
+      <c r="M86" s="138"/>
+      <c r="N86" s="138"/>
+      <c r="O86" s="138"/>
+      <c r="P86" s="139"/>
     </row>
     <row r="87" spans="1:16" ht="17">
       <c r="A87" s="13" t="s">
@@ -11213,10 +11772,10 @@
     </row>
     <row r="104" spans="1:16" ht="17" thickBot="1"/>
     <row r="105" spans="1:16" ht="17" thickTop="1">
-      <c r="A105" s="139" t="s">
+      <c r="A105" s="140" t="s">
         <v>205</v>
       </c>
-      <c r="B105" s="140"/>
+      <c r="B105" s="141"/>
       <c r="C105" s="24"/>
       <c r="D105" s="25"/>
       <c r="E105" s="26"/>
@@ -11233,8 +11792,8 @@
       <c r="P105" s="28"/>
     </row>
     <row r="106" spans="1:16" ht="17" thickBot="1">
-      <c r="A106" s="141"/>
-      <c r="B106" s="142"/>
+      <c r="A106" s="142"/>
+      <c r="B106" s="143"/>
       <c r="C106" s="30"/>
       <c r="D106" s="31"/>
       <c r="E106" s="32"/>
@@ -13584,24 +14143,24 @@
       </c>
     </row>
     <row r="73" spans="1:16" ht="17" thickBot="1">
-      <c r="A73" s="133" t="s">
+      <c r="A73" s="134" t="s">
         <v>288</v>
       </c>
-      <c r="B73" s="134"/>
-      <c r="C73" s="134"/>
-      <c r="D73" s="134"/>
-      <c r="E73" s="134"/>
-      <c r="F73" s="134"/>
-      <c r="G73" s="134"/>
-      <c r="H73" s="134"/>
-      <c r="I73" s="134"/>
-      <c r="J73" s="134"/>
-      <c r="K73" s="134"/>
-      <c r="L73" s="134"/>
-      <c r="M73" s="134"/>
-      <c r="N73" s="134"/>
-      <c r="O73" s="134"/>
-      <c r="P73" s="135"/>
+      <c r="B73" s="135"/>
+      <c r="C73" s="135"/>
+      <c r="D73" s="135"/>
+      <c r="E73" s="135"/>
+      <c r="F73" s="135"/>
+      <c r="G73" s="135"/>
+      <c r="H73" s="135"/>
+      <c r="I73" s="135"/>
+      <c r="J73" s="135"/>
+      <c r="K73" s="135"/>
+      <c r="L73" s="135"/>
+      <c r="M73" s="135"/>
+      <c r="N73" s="135"/>
+      <c r="O73" s="135"/>
+      <c r="P73" s="136"/>
     </row>
     <row r="74" spans="1:16" ht="17">
       <c r="A74" s="13" t="s">
@@ -13809,24 +14368,24 @@
     </row>
     <row r="85" spans="1:16" ht="17" thickBot="1"/>
     <row r="86" spans="1:16" ht="17" thickBot="1">
-      <c r="A86" s="136" t="s">
+      <c r="A86" s="137" t="s">
         <v>208</v>
       </c>
-      <c r="B86" s="137"/>
-      <c r="C86" s="137"/>
-      <c r="D86" s="137"/>
-      <c r="E86" s="137"/>
-      <c r="F86" s="137"/>
-      <c r="G86" s="137"/>
-      <c r="H86" s="137"/>
-      <c r="I86" s="137"/>
-      <c r="J86" s="137"/>
-      <c r="K86" s="137"/>
-      <c r="L86" s="137"/>
-      <c r="M86" s="137"/>
-      <c r="N86" s="137"/>
-      <c r="O86" s="137"/>
-      <c r="P86" s="138"/>
+      <c r="B86" s="138"/>
+      <c r="C86" s="138"/>
+      <c r="D86" s="138"/>
+      <c r="E86" s="138"/>
+      <c r="F86" s="138"/>
+      <c r="G86" s="138"/>
+      <c r="H86" s="138"/>
+      <c r="I86" s="138"/>
+      <c r="J86" s="138"/>
+      <c r="K86" s="138"/>
+      <c r="L86" s="138"/>
+      <c r="M86" s="138"/>
+      <c r="N86" s="138"/>
+      <c r="O86" s="138"/>
+      <c r="P86" s="139"/>
     </row>
     <row r="87" spans="1:16" ht="17">
       <c r="A87" s="13" t="s">
@@ -14249,10 +14808,10 @@
     </row>
     <row r="104" spans="1:16" ht="17" thickBot="1"/>
     <row r="105" spans="1:16" ht="17" thickTop="1">
-      <c r="A105" s="139" t="s">
+      <c r="A105" s="140" t="s">
         <v>205</v>
       </c>
-      <c r="B105" s="140"/>
+      <c r="B105" s="141"/>
       <c r="C105" s="24"/>
       <c r="D105" s="25"/>
       <c r="E105" s="26"/>
@@ -14269,8 +14828,8 @@
       <c r="P105" s="28"/>
     </row>
     <row r="106" spans="1:16" ht="17" thickBot="1">
-      <c r="A106" s="141"/>
-      <c r="B106" s="142"/>
+      <c r="A106" s="142"/>
+      <c r="B106" s="143"/>
       <c r="C106" s="30"/>
       <c r="D106" s="31"/>
       <c r="E106" s="32"/>
@@ -18208,10 +18767,10 @@
         <f>voron2.4_350mm_bom!M1</f>
         <v>Notes</v>
       </c>
-      <c r="Q1" s="143" t="s">
+      <c r="Q1" s="144" t="s">
         <v>135</v>
       </c>
-      <c r="R1" s="144"/>
+      <c r="R1" s="145"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="str">
@@ -21431,18 +21990,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="145"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
+      <c r="J1" s="146"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="19">
       <c r="A2" s="3" t="s">

</xml_diff>

<commit_message>
First successful print. Added the smart filament runout sensor and macros. Had to increase the E-motor current b/c the filament path has a lot of resistance.
</commit_message>
<xml_diff>
--- a/BOM/voron2.4_350mm_bom.xlsx
+++ b/BOM/voron2.4_350mm_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cwilder/Documents/3D Printing/cee-wals/voron-2.4/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1648580-090B-E947-B7B2-E3C0C57DAB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F2BE85-F974-4040-BD35-FDC096D0DEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="500" windowWidth="50420" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="500" windowWidth="50420" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="West3D Voron 2.4 BOM" sheetId="6" r:id="rId1"/>
@@ -1161,7 +1161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2267" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2267" uniqueCount="673">
   <si>
     <t>Category</t>
   </si>
@@ -3301,6 +3301,9 @@
   </si>
   <si>
     <t>vendor: printedsolid.com; Additional filament for printing mods</t>
+  </si>
+  <si>
+    <t>Didn't order for some reason</t>
   </si>
 </sst>
 </file>
@@ -4290,7 +4293,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4652,17 +4655,11 @@
     <xf numFmtId="0" fontId="35" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="39" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="39" borderId="23" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4670,10 +4667,11 @@
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="39" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="39" fillId="39" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="38" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="39" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4719,8 +4717,36 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="38" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="39" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="23" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5128,10 +5154,10 @@
   <dimension ref="A1:AD150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="H76" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="2" topLeftCell="L86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A65" sqref="A65"/>
+      <selection pane="bottomRight" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5158,28 +5184,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="24" customHeight="1">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="138" t="s">
         <v>293</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="139"/>
-      <c r="L1" s="139"/>
-      <c r="M1" s="139"/>
-      <c r="N1" s="139"/>
-      <c r="O1" s="139"/>
-      <c r="P1" s="139"/>
-      <c r="Q1" s="139"/>
-      <c r="R1" s="139"/>
-      <c r="S1" s="139"/>
-      <c r="T1" s="139"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
+      <c r="K1" s="138"/>
+      <c r="L1" s="138"/>
+      <c r="M1" s="138"/>
+      <c r="N1" s="138"/>
+      <c r="O1" s="138"/>
+      <c r="P1" s="138"/>
+      <c r="Q1" s="138"/>
+      <c r="R1" s="138"/>
+      <c r="S1" s="138"/>
+      <c r="T1" s="138"/>
     </row>
     <row r="2" spans="1:30" s="90" customFormat="1" ht="23" customHeight="1" thickBot="1">
       <c r="A2" s="91" t="s">
@@ -5827,59 +5853,59 @@
       <c r="T12" s="98"/>
     </row>
     <row r="13" spans="1:30">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="101" t="s">
         <v>322</v>
       </c>
-      <c r="B13" s="129">
-        <v>1</v>
-      </c>
-      <c r="C13" s="129" t="s">
+      <c r="B13" s="102">
+        <v>1</v>
+      </c>
+      <c r="C13" s="102" t="s">
         <v>298</v>
       </c>
-      <c r="D13" s="129"/>
-      <c r="E13" s="116" t="s">
+      <c r="D13" s="102"/>
+      <c r="E13" s="101" t="s">
         <v>323</v>
       </c>
-      <c r="F13" s="130"/>
-      <c r="G13" s="130"/>
-      <c r="H13" s="133" t="str">
+      <c r="F13" s="103"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="104" t="str">
         <f>E13</f>
         <v>Omron G3NA-210B-DC5 10A SSR</v>
       </c>
-      <c r="I13" s="134"/>
-      <c r="J13" s="117">
+      <c r="I13" s="162"/>
+      <c r="J13" s="106">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="K13" s="121">
+      <c r="K13" s="107">
         <v>28.99</v>
       </c>
-      <c r="L13" s="121">
+      <c r="L13" s="107">
         <f t="shared" si="0"/>
         <v>28.99</v>
       </c>
-      <c r="M13" s="121">
-        <v>0</v>
-      </c>
-      <c r="N13" s="121">
-        <v>0</v>
-      </c>
-      <c r="O13" s="121">
+      <c r="M13" s="107">
+        <v>0</v>
+      </c>
+      <c r="N13" s="107">
+        <v>0</v>
+      </c>
+      <c r="O13" s="107">
         <f t="shared" si="1"/>
         <v>28.99</v>
       </c>
-      <c r="P13" s="121">
+      <c r="P13" s="107">
         <f>O13</f>
         <v>28.99</v>
       </c>
-      <c r="Q13" s="120"/>
-      <c r="R13" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S13" s="123" t="s">
+      <c r="Q13" s="105"/>
+      <c r="R13" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S13" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T13" s="124" t="s">
+      <c r="T13" s="109" t="s">
         <v>553</v>
       </c>
     </row>
@@ -5941,510 +5967,509 @@
       </c>
     </row>
     <row r="15" spans="1:30">
-      <c r="A15" s="116" t="s">
+      <c r="A15" s="101" t="s">
         <v>326</v>
       </c>
-      <c r="B15" s="129">
-        <v>1</v>
-      </c>
-      <c r="C15" s="129" t="s">
+      <c r="B15" s="102">
+        <v>1</v>
+      </c>
+      <c r="C15" s="102" t="s">
         <v>313</v>
       </c>
-      <c r="D15" s="129"/>
-      <c r="E15" s="116" t="s">
+      <c r="D15" s="102"/>
+      <c r="E15" s="101" t="s">
         <v>327</v>
       </c>
-      <c r="F15" s="116" t="s">
+      <c r="F15" s="101" t="s">
         <v>328</v>
       </c>
-      <c r="G15" s="116" t="s">
+      <c r="G15" s="101" t="s">
         <v>329</v>
       </c>
-      <c r="H15" s="133" t="str">
+      <c r="H15" s="104" t="str">
         <f>A15</f>
         <v>Mean Well LRS-200-24 200W 24V 8.8A Power Supply (PSU)</v>
       </c>
-      <c r="I15" s="120"/>
-      <c r="J15" s="117">
+      <c r="I15" s="105"/>
+      <c r="J15" s="106">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="K15" s="121">
+      <c r="K15" s="107">
         <v>30.99</v>
       </c>
-      <c r="L15" s="121">
+      <c r="L15" s="107">
         <f t="shared" si="0"/>
         <v>30.99</v>
       </c>
-      <c r="M15" s="121">
-        <v>0</v>
-      </c>
-      <c r="N15" s="121">
-        <v>0</v>
-      </c>
-      <c r="O15" s="121">
+      <c r="M15" s="107">
+        <v>0</v>
+      </c>
+      <c r="N15" s="107">
+        <v>0</v>
+      </c>
+      <c r="O15" s="107">
         <f t="shared" si="1"/>
         <v>30.99</v>
       </c>
-      <c r="P15" s="121">
+      <c r="P15" s="107">
         <f>O15</f>
         <v>30.99</v>
       </c>
-      <c r="Q15" s="120"/>
-      <c r="R15" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S15" s="123" t="s">
+      <c r="Q15" s="105"/>
+      <c r="R15" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S15" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T15" s="124" t="s">
+      <c r="T15" s="109" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="16" spans="1:30">
-      <c r="A16" s="116" t="s">
+      <c r="A16" s="101" t="s">
         <v>330</v>
       </c>
-      <c r="B16" s="129">
-        <v>1</v>
-      </c>
-      <c r="C16" s="129" t="s">
+      <c r="B16" s="102">
+        <v>1</v>
+      </c>
+      <c r="C16" s="102" t="s">
         <v>313</v>
       </c>
-      <c r="D16" s="129"/>
-      <c r="E16" s="130"/>
-      <c r="F16" s="130"/>
-      <c r="G16" s="130"/>
-      <c r="H16" s="133" t="str">
+      <c r="D16" s="102"/>
+      <c r="E16" s="103"/>
+      <c r="F16" s="103"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="104" t="str">
         <f t="shared" ref="H16:H23" si="4">A16</f>
         <v>Mean Well RS-25-5 25W Power Supply (PSU)</v>
       </c>
-      <c r="I16" s="120"/>
-      <c r="J16" s="117">
+      <c r="I16" s="105"/>
+      <c r="J16" s="106">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="K16" s="121">
+      <c r="K16" s="107">
         <v>18.989999999999998</v>
       </c>
-      <c r="L16" s="121">
+      <c r="L16" s="107">
         <f t="shared" si="0"/>
         <v>18.989999999999998</v>
       </c>
-      <c r="M16" s="121">
-        <v>0</v>
-      </c>
-      <c r="N16" s="121">
-        <v>0</v>
-      </c>
-      <c r="O16" s="121">
+      <c r="M16" s="107">
+        <v>0</v>
+      </c>
+      <c r="N16" s="107">
+        <v>0</v>
+      </c>
+      <c r="O16" s="107">
         <f t="shared" si="1"/>
         <v>18.989999999999998</v>
       </c>
-      <c r="P16" s="121">
+      <c r="P16" s="107">
         <f t="shared" ref="P16:P22" si="5">O16</f>
         <v>18.989999999999998</v>
       </c>
-      <c r="Q16" s="120"/>
-      <c r="R16" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S16" s="123" t="s">
+      <c r="Q16" s="105"/>
+      <c r="R16" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S16" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T16" s="124" t="s">
+      <c r="T16" s="109" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="17" spans="1:30" ht="45">
-      <c r="A17" s="116" t="s">
+      <c r="A17" s="153" t="s">
         <v>331</v>
       </c>
-      <c r="B17" s="129">
-        <v>1</v>
-      </c>
-      <c r="C17" s="129" t="s">
+      <c r="B17" s="154">
+        <v>1</v>
+      </c>
+      <c r="C17" s="154" t="s">
         <v>298</v>
       </c>
-      <c r="D17" s="129"/>
-      <c r="E17" s="116" t="s">
+      <c r="D17" s="154"/>
+      <c r="E17" s="153" t="s">
         <v>332</v>
       </c>
-      <c r="F17" s="130"/>
-      <c r="G17" s="130"/>
-      <c r="H17" s="133" t="str">
+      <c r="F17" s="155"/>
+      <c r="G17" s="155"/>
+      <c r="H17" s="156" t="str">
         <f t="shared" si="4"/>
         <v>ZF - Rocker Switch DPST 16A On-Off - WRG32F2BBRLN</v>
       </c>
-      <c r="I17" s="120"/>
-      <c r="J17" s="117">
+      <c r="I17" s="157" t="s">
+        <v>672</v>
+      </c>
+      <c r="J17" s="158">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="K17" s="121">
+      <c r="K17" s="159">
         <v>2.99</v>
       </c>
-      <c r="L17" s="121">
+      <c r="L17" s="159">
         <f t="shared" si="0"/>
         <v>2.99</v>
       </c>
-      <c r="M17" s="121">
-        <v>0</v>
-      </c>
-      <c r="N17" s="121">
-        <v>0</v>
-      </c>
-      <c r="O17" s="121">
+      <c r="M17" s="159">
+        <v>0</v>
+      </c>
+      <c r="N17" s="159">
+        <v>0</v>
+      </c>
+      <c r="O17" s="159">
         <f t="shared" si="1"/>
         <v>2.99</v>
       </c>
-      <c r="P17" s="121">
-        <f t="shared" si="5"/>
-        <v>2.99</v>
-      </c>
-      <c r="Q17" s="120"/>
-      <c r="R17" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S17" s="123" t="s">
+      <c r="P17" s="159">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="157"/>
+      <c r="R17" s="158"/>
+      <c r="S17" s="160" t="s">
         <v>553</v>
       </c>
-      <c r="T17" s="124" t="s">
+      <c r="T17" s="161" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="18" spans="1:30">
-      <c r="A18" s="116" t="s">
+      <c r="A18" s="101" t="s">
         <v>333</v>
       </c>
-      <c r="B18" s="129">
-        <v>1</v>
-      </c>
-      <c r="C18" s="129"/>
-      <c r="D18" s="129"/>
-      <c r="E18" s="130"/>
-      <c r="F18" s="130"/>
-      <c r="G18" s="130"/>
-      <c r="H18" s="133" t="str">
+      <c r="B18" s="102">
+        <v>1</v>
+      </c>
+      <c r="C18" s="102"/>
+      <c r="D18" s="102"/>
+      <c r="E18" s="103"/>
+      <c r="F18" s="103"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="104" t="str">
         <f t="shared" si="4"/>
         <v>TycoElectronics - 10EHG1-2 Filtered Power Inlet</v>
       </c>
-      <c r="I18" s="120"/>
-      <c r="J18" s="117">
+      <c r="I18" s="105"/>
+      <c r="J18" s="106">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="K18" s="121">
+      <c r="K18" s="107">
         <v>20.99</v>
       </c>
-      <c r="L18" s="121">
+      <c r="L18" s="107">
         <f t="shared" si="0"/>
         <v>20.99</v>
       </c>
-      <c r="M18" s="121">
-        <v>0</v>
-      </c>
-      <c r="N18" s="121">
-        <v>0</v>
-      </c>
-      <c r="O18" s="121">
+      <c r="M18" s="107">
+        <v>0</v>
+      </c>
+      <c r="N18" s="107">
+        <v>0</v>
+      </c>
+      <c r="O18" s="107">
         <f t="shared" si="1"/>
         <v>20.99</v>
       </c>
-      <c r="P18" s="121">
+      <c r="P18" s="107">
         <f t="shared" si="5"/>
         <v>20.99</v>
       </c>
-      <c r="Q18" s="120"/>
-      <c r="R18" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S18" s="123" t="s">
+      <c r="Q18" s="105"/>
+      <c r="R18" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S18" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T18" s="124" t="s">
+      <c r="T18" s="109" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="19" spans="1:30">
-      <c r="A19" s="116" t="s">
+      <c r="A19" s="101" t="s">
         <v>292</v>
       </c>
-      <c r="B19" s="129">
+      <c r="B19" s="102">
         <v>3</v>
       </c>
-      <c r="C19" s="129" t="s">
+      <c r="C19" s="102" t="s">
         <v>313</v>
       </c>
-      <c r="D19" s="129"/>
-      <c r="E19" s="130"/>
-      <c r="F19" s="130"/>
-      <c r="G19" s="130"/>
-      <c r="H19" s="133" t="str">
+      <c r="D19" s="102"/>
+      <c r="E19" s="103"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="103"/>
+      <c r="H19" s="104" t="str">
         <f t="shared" si="4"/>
         <v>Fuse 8A 250V Holder Cartridge 5 X 20mm Glass</v>
       </c>
-      <c r="I19" s="120"/>
-      <c r="J19" s="117">
+      <c r="I19" s="105"/>
+      <c r="J19" s="106">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="K19" s="121">
+      <c r="K19" s="107">
         <v>0.99</v>
       </c>
-      <c r="L19" s="121">
+      <c r="L19" s="107">
         <f t="shared" si="0"/>
         <v>2.9699999999999998</v>
       </c>
-      <c r="M19" s="121">
-        <v>0</v>
-      </c>
-      <c r="N19" s="121">
-        <v>0</v>
-      </c>
-      <c r="O19" s="121">
+      <c r="M19" s="107">
+        <v>0</v>
+      </c>
+      <c r="N19" s="107">
+        <v>0</v>
+      </c>
+      <c r="O19" s="107">
         <f t="shared" si="1"/>
         <v>2.9699999999999998</v>
       </c>
-      <c r="P19" s="121">
+      <c r="P19" s="107">
         <f t="shared" si="5"/>
         <v>2.9699999999999998</v>
       </c>
-      <c r="Q19" s="120"/>
-      <c r="R19" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S19" s="123" t="s">
+      <c r="Q19" s="105"/>
+      <c r="R19" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S19" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T19" s="124" t="s">
+      <c r="T19" s="109" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="20" spans="1:30">
-      <c r="A20" s="116" t="s">
+      <c r="A20" s="101" t="s">
         <v>334</v>
       </c>
-      <c r="B20" s="129">
-        <v>1</v>
-      </c>
-      <c r="C20" s="129" t="s">
+      <c r="B20" s="102">
+        <v>1</v>
+      </c>
+      <c r="C20" s="102" t="s">
         <v>298</v>
       </c>
-      <c r="D20" s="129"/>
-      <c r="E20" s="116" t="s">
+      <c r="D20" s="102"/>
+      <c r="E20" s="101" t="s">
         <v>335</v>
       </c>
-      <c r="F20" s="130"/>
-      <c r="G20" s="130"/>
-      <c r="H20" s="133" t="str">
+      <c r="F20" s="103"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="104" t="str">
         <f t="shared" si="4"/>
         <v>GDSTIME DC 24V 40x40x10 Axial Fan GDA4010</v>
       </c>
-      <c r="I20" s="120" t="s">
+      <c r="I20" s="105" t="s">
         <v>557</v>
       </c>
-      <c r="J20" s="117">
+      <c r="J20" s="106">
         <v>2</v>
       </c>
-      <c r="K20" s="121">
+      <c r="K20" s="107">
         <v>6.99</v>
       </c>
-      <c r="L20" s="121">
+      <c r="L20" s="107">
         <f t="shared" si="0"/>
         <v>13.98</v>
       </c>
-      <c r="M20" s="121">
-        <v>0</v>
-      </c>
-      <c r="N20" s="121">
-        <v>0</v>
-      </c>
-      <c r="O20" s="121">
+      <c r="M20" s="107">
+        <v>0</v>
+      </c>
+      <c r="N20" s="107">
+        <v>0</v>
+      </c>
+      <c r="O20" s="107">
         <f t="shared" si="1"/>
         <v>13.98</v>
       </c>
-      <c r="P20" s="121">
+      <c r="P20" s="107">
         <f t="shared" si="5"/>
         <v>13.98</v>
       </c>
-      <c r="Q20" s="120"/>
-      <c r="R20" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S20" s="123" t="s">
+      <c r="Q20" s="105"/>
+      <c r="R20" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S20" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T20" s="124" t="s">
+      <c r="T20" s="109" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="21" spans="1:30">
-      <c r="A21" s="116" t="s">
+      <c r="A21" s="101" t="s">
         <v>336</v>
       </c>
-      <c r="B21" s="129">
-        <v>1</v>
-      </c>
-      <c r="C21" s="129" t="s">
+      <c r="B21" s="102">
+        <v>1</v>
+      </c>
+      <c r="C21" s="102" t="s">
         <v>313</v>
       </c>
-      <c r="D21" s="129"/>
-      <c r="E21" s="130"/>
-      <c r="F21" s="130"/>
-      <c r="G21" s="130"/>
-      <c r="H21" s="133" t="str">
+      <c r="D21" s="102"/>
+      <c r="E21" s="103"/>
+      <c r="F21" s="103"/>
+      <c r="G21" s="103"/>
+      <c r="H21" s="104" t="str">
         <f t="shared" si="4"/>
         <v>GDSTIME DC 24V 40x40x20 Centrifugal Blower Fan GDB4020</v>
       </c>
-      <c r="I21" s="120"/>
-      <c r="J21" s="117">
+      <c r="I21" s="105"/>
+      <c r="J21" s="106">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="K21" s="121">
+      <c r="K21" s="107">
         <v>6.99</v>
       </c>
-      <c r="L21" s="121">
+      <c r="L21" s="107">
         <f t="shared" si="0"/>
         <v>6.99</v>
       </c>
-      <c r="M21" s="121">
-        <v>0</v>
-      </c>
-      <c r="N21" s="121">
-        <v>0</v>
-      </c>
-      <c r="O21" s="121">
+      <c r="M21" s="107">
+        <v>0</v>
+      </c>
+      <c r="N21" s="107">
+        <v>0</v>
+      </c>
+      <c r="O21" s="107">
         <f t="shared" si="1"/>
         <v>6.99</v>
       </c>
-      <c r="P21" s="121">
+      <c r="P21" s="107">
         <f t="shared" si="5"/>
         <v>6.99</v>
       </c>
-      <c r="Q21" s="120"/>
-      <c r="R21" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S21" s="123" t="s">
+      <c r="Q21" s="105"/>
+      <c r="R21" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S21" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T21" s="124" t="s">
+      <c r="T21" s="109" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="22" spans="1:30" ht="30">
-      <c r="A22" s="116" t="s">
+      <c r="A22" s="101" t="s">
         <v>337</v>
       </c>
-      <c r="B22" s="129">
+      <c r="B22" s="102">
         <v>3</v>
       </c>
-      <c r="C22" s="129" t="s">
+      <c r="C22" s="102" t="s">
         <v>313</v>
       </c>
-      <c r="D22" s="129"/>
-      <c r="E22" s="130"/>
-      <c r="F22" s="130"/>
-      <c r="G22" s="130"/>
-      <c r="H22" s="133" t="str">
+      <c r="D22" s="102"/>
+      <c r="E22" s="103"/>
+      <c r="F22" s="103"/>
+      <c r="G22" s="103"/>
+      <c r="H22" s="104" t="str">
         <f t="shared" si="4"/>
         <v>GDSTIME DC 24V 60x60x20 Axial Fan GDA6020 Dual Ball Bearing 5000RPM 1.7W 0.1A XH2.54</v>
       </c>
-      <c r="I22" s="120"/>
-      <c r="J22" s="117">
+      <c r="I22" s="105"/>
+      <c r="J22" s="106">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="K22" s="121">
+      <c r="K22" s="107">
         <v>6.99</v>
       </c>
-      <c r="L22" s="121">
+      <c r="L22" s="107">
         <f t="shared" si="0"/>
         <v>20.97</v>
       </c>
-      <c r="M22" s="121">
-        <v>0</v>
-      </c>
-      <c r="N22" s="121">
-        <v>0</v>
-      </c>
-      <c r="O22" s="121">
+      <c r="M22" s="107">
+        <v>0</v>
+      </c>
+      <c r="N22" s="107">
+        <v>0</v>
+      </c>
+      <c r="O22" s="107">
         <f t="shared" si="1"/>
         <v>20.97</v>
       </c>
-      <c r="P22" s="121">
+      <c r="P22" s="107">
         <f t="shared" si="5"/>
         <v>20.97</v>
       </c>
-      <c r="Q22" s="120"/>
-      <c r="R22" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S22" s="123" t="s">
+      <c r="Q22" s="105"/>
+      <c r="R22" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S22" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T22" s="124" t="s">
+      <c r="T22" s="109" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="23" spans="1:30">
-      <c r="A23" s="116" t="s">
+      <c r="A23" s="101" t="s">
         <v>338</v>
       </c>
-      <c r="B23" s="129">
-        <v>1</v>
-      </c>
-      <c r="C23" s="129" t="s">
+      <c r="B23" s="102">
+        <v>1</v>
+      </c>
+      <c r="C23" s="102" t="s">
         <v>313</v>
       </c>
-      <c r="D23" s="129"/>
-      <c r="E23" s="130"/>
-      <c r="F23" s="130"/>
-      <c r="G23" s="130"/>
-      <c r="H23" s="133" t="str">
+      <c r="D23" s="102"/>
+      <c r="E23" s="103"/>
+      <c r="F23" s="103"/>
+      <c r="G23" s="103"/>
+      <c r="H23" s="104" t="str">
         <f t="shared" si="4"/>
         <v>125C Cutoff 15A Thermal Fuse</v>
       </c>
-      <c r="I23" s="120" t="s">
+      <c r="I23" s="105" t="s">
         <v>543</v>
       </c>
-      <c r="J23" s="117">
+      <c r="J23" s="106">
         <v>2</v>
       </c>
-      <c r="K23" s="121">
+      <c r="K23" s="107">
         <v>1.29</v>
       </c>
-      <c r="L23" s="121">
+      <c r="L23" s="107">
         <f t="shared" si="0"/>
         <v>2.58</v>
       </c>
-      <c r="M23" s="121">
-        <v>0</v>
-      </c>
-      <c r="N23" s="121">
-        <v>0</v>
-      </c>
-      <c r="O23" s="121">
+      <c r="M23" s="107">
+        <v>0</v>
+      </c>
+      <c r="N23" s="107">
+        <v>0</v>
+      </c>
+      <c r="O23" s="107">
         <f t="shared" si="1"/>
         <v>2.58</v>
       </c>
-      <c r="P23" s="121">
+      <c r="P23" s="107">
         <f>O23</f>
         <v>2.58</v>
       </c>
-      <c r="Q23" s="122">
+      <c r="Q23" s="114">
         <f>-1*K23</f>
         <v>-1.29</v>
       </c>
-      <c r="R23" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S23" s="123" t="s">
+      <c r="R23" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S23" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T23" s="124" t="s">
+      <c r="T23" s="109" t="s">
         <v>553</v>
       </c>
     </row>
@@ -6682,61 +6707,61 @@
       </c>
     </row>
     <row r="28" spans="1:30">
-      <c r="A28" s="132" t="s">
+      <c r="A28" s="126" t="s">
         <v>385</v>
       </c>
-      <c r="B28" s="129">
+      <c r="B28" s="102">
         <v>7</v>
       </c>
-      <c r="C28" s="129" t="s">
+      <c r="C28" s="102" t="s">
         <v>298</v>
       </c>
-      <c r="D28" s="129"/>
-      <c r="E28" s="116" t="s">
+      <c r="D28" s="102"/>
+      <c r="E28" s="101" t="s">
         <v>386</v>
       </c>
-      <c r="F28" s="130" t="s">
+      <c r="F28" s="103" t="s">
         <v>343</v>
       </c>
-      <c r="G28" s="130"/>
-      <c r="H28" s="133" t="str">
+      <c r="G28" s="103"/>
+      <c r="H28" s="104" t="str">
         <f>E28</f>
         <v>TMC2226</v>
       </c>
-      <c r="I28" s="120"/>
-      <c r="J28" s="117">
+      <c r="I28" s="105"/>
+      <c r="J28" s="106">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="K28" s="121">
+      <c r="K28" s="107">
         <v>6.49</v>
       </c>
-      <c r="L28" s="121">
+      <c r="L28" s="107">
         <f t="shared" si="0"/>
         <v>45.43</v>
       </c>
-      <c r="M28" s="121">
-        <v>0</v>
-      </c>
-      <c r="N28" s="121">
-        <v>0</v>
-      </c>
-      <c r="O28" s="121">
+      <c r="M28" s="107">
+        <v>0</v>
+      </c>
+      <c r="N28" s="107">
+        <v>0</v>
+      </c>
+      <c r="O28" s="107">
         <f t="shared" si="1"/>
         <v>45.43</v>
       </c>
-      <c r="P28" s="121">
+      <c r="P28" s="107">
         <f>O28</f>
         <v>45.43</v>
       </c>
-      <c r="Q28" s="122"/>
-      <c r="R28" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S28" s="123" t="s">
+      <c r="Q28" s="114"/>
+      <c r="R28" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S28" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T28" s="124" t="s">
+      <c r="T28" s="109" t="s">
         <v>553</v>
       </c>
     </row>
@@ -6760,7 +6785,7 @@
       <c r="G29" s="116" t="s">
         <v>634</v>
       </c>
-      <c r="H29" s="133" t="str">
+      <c r="H29" s="132" t="str">
         <f>G29</f>
         <v>BTT HDMI7 V1.0 Display from DFH</v>
       </c>
@@ -6967,57 +6992,57 @@
       <c r="T32" s="98"/>
     </row>
     <row r="33" spans="1:20">
-      <c r="A33" s="116" t="s">
+      <c r="A33" s="101" t="s">
         <v>346</v>
       </c>
-      <c r="B33" s="129">
+      <c r="B33" s="102">
         <v>8</v>
       </c>
-      <c r="C33" s="129" t="s">
+      <c r="C33" s="102" t="s">
         <v>313</v>
       </c>
-      <c r="D33" s="129"/>
-      <c r="E33" s="130"/>
-      <c r="F33" s="130"/>
-      <c r="G33" s="130"/>
-      <c r="H33" s="131" t="str">
+      <c r="D33" s="102"/>
+      <c r="E33" s="103"/>
+      <c r="F33" s="103"/>
+      <c r="G33" s="103"/>
+      <c r="H33" s="110" t="str">
         <f>A33</f>
         <v>6mm x 3mm Round Neomydium Magnets</v>
       </c>
-      <c r="I33" s="120" t="s">
+      <c r="I33" s="105" t="s">
         <v>542</v>
       </c>
-      <c r="J33" s="117">
+      <c r="J33" s="106">
         <v>16</v>
       </c>
-      <c r="K33" s="121">
+      <c r="K33" s="107">
         <v>0.49</v>
       </c>
-      <c r="L33" s="121">
+      <c r="L33" s="107">
         <f t="shared" si="0"/>
         <v>7.84</v>
       </c>
-      <c r="M33" s="121"/>
-      <c r="N33" s="121"/>
-      <c r="O33" s="121">
+      <c r="M33" s="107"/>
+      <c r="N33" s="107"/>
+      <c r="O33" s="107">
         <f t="shared" si="1"/>
         <v>7.84</v>
       </c>
-      <c r="P33" s="121">
+      <c r="P33" s="107">
         <f>O33</f>
         <v>7.84</v>
       </c>
-      <c r="Q33" s="122">
+      <c r="Q33" s="114">
         <f>-1*(K33*8)</f>
         <v>-3.92</v>
       </c>
-      <c r="R33" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S33" s="123" t="s">
+      <c r="R33" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S33" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T33" s="124" t="s">
+      <c r="T33" s="109" t="s">
         <v>553</v>
       </c>
     </row>
@@ -7106,179 +7131,179 @@
       <c r="T35" s="98"/>
     </row>
     <row r="36" spans="1:20" ht="30">
-      <c r="A36" s="132" t="s">
+      <c r="A36" s="126" t="s">
         <v>349</v>
       </c>
-      <c r="B36" s="129">
-        <v>1</v>
-      </c>
-      <c r="C36" s="129" t="s">
+      <c r="B36" s="102">
+        <v>1</v>
+      </c>
+      <c r="C36" s="102" t="s">
         <v>298</v>
       </c>
-      <c r="D36" s="129"/>
-      <c r="E36" s="116" t="s">
+      <c r="D36" s="102"/>
+      <c r="E36" s="101" t="s">
         <v>350</v>
       </c>
-      <c r="F36" s="130"/>
-      <c r="G36" s="130"/>
-      <c r="H36" s="131" t="str">
+      <c r="F36" s="103"/>
+      <c r="G36" s="103"/>
+      <c r="H36" s="110" t="str">
         <f>E36</f>
         <v>BMG Components Kit Nano Coated RNC</v>
       </c>
-      <c r="I36" s="120"/>
-      <c r="J36" s="117">
+      <c r="I36" s="105"/>
+      <c r="J36" s="106">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="K36" s="121">
+      <c r="K36" s="107">
         <v>32.99</v>
       </c>
-      <c r="L36" s="121">
+      <c r="L36" s="107">
         <f t="shared" si="0"/>
         <v>32.99</v>
       </c>
-      <c r="M36" s="121">
-        <v>0</v>
-      </c>
-      <c r="N36" s="121">
-        <v>0</v>
-      </c>
-      <c r="O36" s="121">
+      <c r="M36" s="107">
+        <v>0</v>
+      </c>
+      <c r="N36" s="107">
+        <v>0</v>
+      </c>
+      <c r="O36" s="107">
         <f t="shared" si="1"/>
         <v>32.99</v>
       </c>
-      <c r="P36" s="121">
+      <c r="P36" s="107">
         <f>O36</f>
         <v>32.99</v>
       </c>
-      <c r="Q36" s="122"/>
-      <c r="R36" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S36" s="123" t="s">
+      <c r="Q36" s="114"/>
+      <c r="R36" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S36" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T36" s="124" t="s">
+      <c r="T36" s="109" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="30">
-      <c r="A37" s="116" t="s">
+      <c r="A37" s="101" t="s">
         <v>351</v>
       </c>
-      <c r="B37" s="129">
-        <v>1</v>
-      </c>
-      <c r="C37" s="129" t="s">
+      <c r="B37" s="102">
+        <v>1</v>
+      </c>
+      <c r="C37" s="102" t="s">
         <v>298</v>
       </c>
-      <c r="D37" s="129"/>
-      <c r="E37" s="116" t="s">
+      <c r="D37" s="102"/>
+      <c r="E37" s="101" t="s">
         <v>352</v>
       </c>
-      <c r="F37" s="130" t="s">
+      <c r="F37" s="103" t="s">
         <v>353</v>
       </c>
-      <c r="G37" s="130"/>
-      <c r="H37" s="131" t="str">
+      <c r="G37" s="103"/>
+      <c r="H37" s="110" t="str">
         <f>A37</f>
         <v>Wiring Harness for Voron 2.4 / Trident</v>
       </c>
-      <c r="I37" s="120" t="s">
+      <c r="I37" s="105" t="s">
         <v>396</v>
       </c>
-      <c r="J37" s="117">
+      <c r="J37" s="106">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="K37" s="121">
+      <c r="K37" s="107">
         <v>79.989999999999995</v>
       </c>
-      <c r="L37" s="121">
+      <c r="L37" s="107">
         <f t="shared" si="0"/>
         <v>79.989999999999995</v>
       </c>
-      <c r="M37" s="121">
-        <v>0</v>
-      </c>
-      <c r="N37" s="121">
-        <v>0</v>
-      </c>
-      <c r="O37" s="121">
+      <c r="M37" s="107">
+        <v>0</v>
+      </c>
+      <c r="N37" s="107">
+        <v>0</v>
+      </c>
+      <c r="O37" s="107">
         <f t="shared" si="1"/>
         <v>79.989999999999995</v>
       </c>
-      <c r="P37" s="121">
+      <c r="P37" s="107">
         <f t="shared" ref="P37:P38" si="12">O37</f>
         <v>79.989999999999995</v>
       </c>
-      <c r="Q37" s="122"/>
-      <c r="R37" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S37" s="123" t="s">
+      <c r="Q37" s="114"/>
+      <c r="R37" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S37" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T37" s="124" t="s">
+      <c r="T37" s="109" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="38" spans="1:20" ht="30">
-      <c r="A38" s="116" t="s">
+      <c r="A38" s="101" t="s">
         <v>394</v>
       </c>
-      <c r="B38" s="129">
-        <v>1</v>
-      </c>
-      <c r="C38" s="129" t="s">
+      <c r="B38" s="102">
+        <v>1</v>
+      </c>
+      <c r="C38" s="102" t="s">
         <v>298</v>
       </c>
-      <c r="D38" s="129"/>
-      <c r="E38" s="116" t="s">
+      <c r="D38" s="102"/>
+      <c r="E38" s="101" t="s">
         <v>393</v>
       </c>
-      <c r="F38" s="130"/>
-      <c r="G38" s="130"/>
-      <c r="H38" s="131" t="str">
+      <c r="F38" s="103"/>
+      <c r="G38" s="103"/>
+      <c r="H38" s="110" t="str">
         <f>E38</f>
         <v>IGUS Cable Chain Set (350mm)</v>
       </c>
-      <c r="I38" s="120" t="s">
+      <c r="I38" s="105" t="s">
         <v>395</v>
       </c>
-      <c r="J38" s="117">
+      <c r="J38" s="106">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="K38" s="121">
+      <c r="K38" s="107">
         <v>79.989999999999995</v>
       </c>
-      <c r="L38" s="121">
+      <c r="L38" s="107">
         <f t="shared" si="0"/>
         <v>79.989999999999995</v>
       </c>
-      <c r="M38" s="121">
-        <v>0</v>
-      </c>
-      <c r="N38" s="121">
-        <v>0</v>
-      </c>
-      <c r="O38" s="121">
+      <c r="M38" s="107">
+        <v>0</v>
+      </c>
+      <c r="N38" s="107">
+        <v>0</v>
+      </c>
+      <c r="O38" s="107">
         <f t="shared" si="1"/>
         <v>79.989999999999995</v>
       </c>
-      <c r="P38" s="121">
+      <c r="P38" s="107">
         <f t="shared" si="12"/>
         <v>79.989999999999995</v>
       </c>
-      <c r="Q38" s="120"/>
-      <c r="R38" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S38" s="123" t="s">
+      <c r="Q38" s="105"/>
+      <c r="R38" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S38" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T38" s="124" t="s">
+      <c r="T38" s="109" t="s">
         <v>553</v>
       </c>
     </row>
@@ -7534,8 +7559,8 @@
         <v>298</v>
       </c>
       <c r="D43" s="129"/>
-      <c r="E43" s="132"/>
-      <c r="F43" s="132"/>
+      <c r="E43" s="131"/>
+      <c r="F43" s="131"/>
       <c r="G43" s="130"/>
       <c r="H43" s="119" t="str">
         <f>A43</f>
@@ -7582,63 +7607,63 @@
       </c>
     </row>
     <row r="44" spans="1:20" ht="30">
-      <c r="A44" s="132" t="s">
+      <c r="A44" s="126" t="s">
         <v>356</v>
       </c>
-      <c r="B44" s="129">
-        <v>1</v>
-      </c>
-      <c r="C44" s="129" t="s">
+      <c r="B44" s="102">
+        <v>1</v>
+      </c>
+      <c r="C44" s="102" t="s">
         <v>298</v>
       </c>
-      <c r="D44" s="129"/>
-      <c r="E44" s="132" t="s">
+      <c r="D44" s="102"/>
+      <c r="E44" s="126" t="s">
         <v>357</v>
       </c>
-      <c r="F44" s="132" t="s">
+      <c r="F44" s="126" t="s">
         <v>358</v>
       </c>
-      <c r="G44" s="116" t="s">
+      <c r="G44" s="101" t="s">
         <v>406</v>
       </c>
-      <c r="H44" s="119" t="str">
+      <c r="H44" s="112" t="str">
         <f>G44</f>
         <v>Phaetus Rapido UHF /TL PT1000 (black)</v>
       </c>
-      <c r="I44" s="120"/>
-      <c r="J44" s="117">
+      <c r="I44" s="105"/>
+      <c r="J44" s="106">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="K44" s="121">
+      <c r="K44" s="107">
         <v>119.99</v>
       </c>
-      <c r="L44" s="121">
+      <c r="L44" s="107">
         <f t="shared" si="0"/>
         <v>119.99</v>
       </c>
-      <c r="M44" s="121">
-        <v>0</v>
-      </c>
-      <c r="N44" s="121">
-        <v>0</v>
-      </c>
-      <c r="O44" s="121">
+      <c r="M44" s="107">
+        <v>0</v>
+      </c>
+      <c r="N44" s="107">
+        <v>0</v>
+      </c>
+      <c r="O44" s="107">
         <f t="shared" si="1"/>
         <v>119.99</v>
       </c>
-      <c r="P44" s="121">
+      <c r="P44" s="107">
         <f t="shared" si="13"/>
         <v>119.99</v>
       </c>
-      <c r="Q44" s="120"/>
-      <c r="R44" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S44" s="123" t="s">
+      <c r="Q44" s="105"/>
+      <c r="R44" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S44" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T44" s="124" t="s">
+      <c r="T44" s="109" t="s">
         <v>553</v>
       </c>
     </row>
@@ -8030,61 +8055,61 @@
       <c r="T52" s="98"/>
     </row>
     <row r="53" spans="1:20">
-      <c r="A53" s="116" t="s">
+      <c r="A53" s="101" t="s">
         <v>412</v>
       </c>
-      <c r="B53" s="129">
+      <c r="B53" s="102">
         <v>2</v>
       </c>
-      <c r="C53" s="129" t="s">
+      <c r="C53" s="102" t="s">
         <v>313</v>
       </c>
-      <c r="D53" s="129"/>
-      <c r="E53" s="130"/>
-      <c r="F53" s="130"/>
-      <c r="G53" s="130"/>
-      <c r="H53" s="119" t="str">
+      <c r="D53" s="102"/>
+      <c r="E53" s="103"/>
+      <c r="F53" s="103"/>
+      <c r="G53" s="103"/>
+      <c r="H53" s="112" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">3-3 DIN Mounting Fast Wire Cable Connectors / Wago Connector </v>
       </c>
-      <c r="I53" s="120" t="s">
+      <c r="I53" s="105" t="s">
         <v>555</v>
       </c>
-      <c r="J53" s="117">
+      <c r="J53" s="106">
         <v>3</v>
       </c>
-      <c r="K53" s="121">
+      <c r="K53" s="107">
         <v>3.49</v>
       </c>
-      <c r="L53" s="121">
+      <c r="L53" s="107">
         <f t="shared" si="15"/>
         <v>10.47</v>
       </c>
-      <c r="M53" s="121">
-        <v>0</v>
-      </c>
-      <c r="N53" s="121">
-        <v>0</v>
-      </c>
-      <c r="O53" s="121">
+      <c r="M53" s="107">
+        <v>0</v>
+      </c>
+      <c r="N53" s="107">
+        <v>0</v>
+      </c>
+      <c r="O53" s="107">
         <f>L53+M53+N53</f>
         <v>10.47</v>
       </c>
-      <c r="P53" s="121">
+      <c r="P53" s="107">
         <f>O53</f>
         <v>10.47</v>
       </c>
-      <c r="Q53" s="122">
+      <c r="Q53" s="114">
         <f>-1*K53</f>
         <v>-3.49</v>
       </c>
-      <c r="R53" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S53" s="123" t="s">
+      <c r="R53" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S53" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T53" s="124" t="s">
+      <c r="T53" s="109" t="s">
         <v>553</v>
       </c>
     </row>
@@ -8154,7 +8179,7 @@
         <v>67</v>
       </c>
       <c r="B55" s="66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55" s="66" t="s">
         <v>313</v>
@@ -8172,7 +8197,7 @@
       </c>
       <c r="J55" s="63">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K55" s="64"/>
       <c r="L55" s="64">
@@ -8196,7 +8221,7 @@
         <v>367</v>
       </c>
       <c r="B56" s="66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C56" s="66" t="s">
         <v>313</v>
@@ -8211,7 +8236,7 @@
       </c>
       <c r="J56" s="63">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K56" s="64"/>
       <c r="L56" s="64">
@@ -8244,7 +8269,7 @@
       <c r="E57" s="118"/>
       <c r="F57" s="118"/>
       <c r="G57" s="130"/>
-      <c r="H57" s="138" t="str">
+      <c r="H57" s="135" t="str">
         <f>A57</f>
         <v>3M VHB Tape 5952 5mm width</v>
       </c>
@@ -8302,7 +8327,7 @@
       <c r="E58" s="118"/>
       <c r="F58" s="118"/>
       <c r="G58" s="130"/>
-      <c r="H58" s="138" t="str">
+      <c r="H58" s="135" t="str">
         <f>A58</f>
         <v>3M VHB Tape 5952 6.35mm width</v>
       </c>
@@ -8556,7 +8581,7 @@
         <v>446</v>
       </c>
       <c r="B63" s="63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C63" s="63" t="s">
         <v>313</v>
@@ -8574,20 +8599,20 @@
       </c>
       <c r="J63" s="63">
         <f t="shared" si="21"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K63" s="64">
         <v>4</v>
       </c>
       <c r="L63" s="64">
         <f t="shared" si="19"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M63" s="64"/>
       <c r="N63" s="64"/>
       <c r="O63" s="64">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P63" s="64"/>
       <c r="Q63" s="75"/>
@@ -9574,179 +9599,179 @@
       <c r="T80" s="98"/>
     </row>
     <row r="81" spans="1:20" ht="30">
-      <c r="A81" s="116" t="s">
+      <c r="A81" s="101" t="s">
         <v>549</v>
       </c>
-      <c r="B81" s="117">
-        <v>1</v>
-      </c>
-      <c r="C81" s="117" t="s">
+      <c r="B81" s="106">
+        <v>1</v>
+      </c>
+      <c r="C81" s="106" t="s">
         <v>313</v>
       </c>
-      <c r="D81" s="117" t="s">
+      <c r="D81" s="106" t="s">
         <v>298</v>
       </c>
-      <c r="E81" s="118"/>
-      <c r="F81" s="118"/>
-      <c r="G81" s="118"/>
-      <c r="H81" s="119" t="str">
+      <c r="E81" s="111"/>
+      <c r="F81" s="111"/>
+      <c r="G81" s="111"/>
+      <c r="H81" s="112" t="str">
         <f t="shared" ref="H81:H89" si="48">A81</f>
         <v>LDO Nema14 36mm Pancake Stepper Motor LDO-36STH20-1004AHG</v>
       </c>
-      <c r="I81" s="120" t="s">
+      <c r="I81" s="105" t="s">
         <v>499</v>
       </c>
-      <c r="J81" s="117">
+      <c r="J81" s="106">
         <f t="shared" si="45"/>
         <v>1</v>
       </c>
-      <c r="K81" s="121">
+      <c r="K81" s="107">
         <v>20.99</v>
       </c>
-      <c r="L81" s="121">
+      <c r="L81" s="107">
         <f t="shared" si="46"/>
         <v>20.99</v>
       </c>
-      <c r="M81" s="121">
-        <v>0</v>
-      </c>
-      <c r="N81" s="121">
-        <v>0</v>
-      </c>
-      <c r="O81" s="121">
+      <c r="M81" s="107">
+        <v>0</v>
+      </c>
+      <c r="N81" s="107">
+        <v>0</v>
+      </c>
+      <c r="O81" s="107">
         <f t="shared" si="47"/>
         <v>20.99</v>
       </c>
-      <c r="P81" s="121">
+      <c r="P81" s="107">
         <f t="shared" ref="P81:P91" si="49">O81</f>
         <v>20.99</v>
       </c>
-      <c r="Q81" s="120"/>
-      <c r="R81" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S81" s="123" t="s">
+      <c r="Q81" s="105"/>
+      <c r="R81" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S81" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T81" s="124" t="s">
+      <c r="T81" s="109" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="82" spans="1:20" ht="30">
-      <c r="A82" s="116" t="s">
+      <c r="A82" s="101" t="s">
         <v>554</v>
       </c>
-      <c r="B82" s="117">
-        <v>1</v>
-      </c>
-      <c r="C82" s="117" t="s">
+      <c r="B82" s="106">
+        <v>1</v>
+      </c>
+      <c r="C82" s="106" t="s">
         <v>313</v>
       </c>
-      <c r="D82" s="117" t="s">
+      <c r="D82" s="106" t="s">
         <v>298</v>
       </c>
-      <c r="E82" s="118"/>
-      <c r="F82" s="118"/>
-      <c r="G82" s="118"/>
-      <c r="H82" s="119" t="str">
+      <c r="E82" s="111"/>
+      <c r="F82" s="111"/>
+      <c r="G82" s="111"/>
+      <c r="H82" s="112" t="str">
         <f t="shared" si="48"/>
         <v>Hartk Stealthburner Toolhead PCB</v>
       </c>
-      <c r="I82" s="120" t="s">
+      <c r="I82" s="105" t="s">
         <v>499</v>
       </c>
-      <c r="J82" s="117">
+      <c r="J82" s="106">
         <f t="shared" si="45"/>
         <v>1</v>
       </c>
-      <c r="K82" s="121">
+      <c r="K82" s="107">
         <v>21.99</v>
       </c>
-      <c r="L82" s="121">
+      <c r="L82" s="107">
         <f t="shared" si="46"/>
         <v>21.99</v>
       </c>
-      <c r="M82" s="121">
-        <v>0</v>
-      </c>
-      <c r="N82" s="121">
-        <v>0</v>
-      </c>
-      <c r="O82" s="121">
+      <c r="M82" s="107">
+        <v>0</v>
+      </c>
+      <c r="N82" s="107">
+        <v>0</v>
+      </c>
+      <c r="O82" s="107">
         <f t="shared" si="47"/>
         <v>21.99</v>
       </c>
-      <c r="P82" s="121">
+      <c r="P82" s="107">
         <f t="shared" si="49"/>
         <v>21.99</v>
       </c>
-      <c r="Q82" s="120"/>
-      <c r="R82" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S82" s="123" t="s">
+      <c r="Q82" s="105"/>
+      <c r="R82" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S82" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T82" s="124" t="s">
+      <c r="T82" s="109" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="83" spans="1:20" ht="30">
-      <c r="A83" s="116" t="s">
+      <c r="A83" s="101" t="s">
         <v>556</v>
       </c>
-      <c r="B83" s="117">
-        <v>1</v>
-      </c>
-      <c r="C83" s="117" t="s">
+      <c r="B83" s="106">
+        <v>1</v>
+      </c>
+      <c r="C83" s="106" t="s">
         <v>313</v>
       </c>
-      <c r="D83" s="117" t="s">
+      <c r="D83" s="106" t="s">
         <v>298</v>
       </c>
-      <c r="E83" s="118"/>
-      <c r="F83" s="118"/>
-      <c r="G83" s="118"/>
-      <c r="H83" s="119" t="str">
+      <c r="E83" s="111"/>
+      <c r="F83" s="111"/>
+      <c r="G83" s="111"/>
+      <c r="H83" s="112" t="str">
         <f t="shared" si="48"/>
         <v>5015 GDSTIME DC 24V 50x50x15 Centrifugal Blower Fan GDB5015Dual Ball Bearing 6000RPM 2.2W .1A XH2.54</v>
       </c>
-      <c r="I83" s="120" t="s">
+      <c r="I83" s="105" t="s">
         <v>499</v>
       </c>
-      <c r="J83" s="117">
+      <c r="J83" s="106">
         <f t="shared" ref="J83:J85" si="50">B83</f>
         <v>1</v>
       </c>
-      <c r="K83" s="121">
+      <c r="K83" s="107">
         <v>8.99</v>
       </c>
-      <c r="L83" s="121">
+      <c r="L83" s="107">
         <f t="shared" ref="L83:L85" si="51">J83*K83</f>
         <v>8.99</v>
       </c>
-      <c r="M83" s="121">
-        <v>0</v>
-      </c>
-      <c r="N83" s="121">
-        <v>0</v>
-      </c>
-      <c r="O83" s="121">
+      <c r="M83" s="107">
+        <v>0</v>
+      </c>
+      <c r="N83" s="107">
+        <v>0</v>
+      </c>
+      <c r="O83" s="107">
         <f t="shared" ref="O83:O85" si="52">L83+M83+N83</f>
         <v>8.99</v>
       </c>
-      <c r="P83" s="121">
+      <c r="P83" s="107">
         <f t="shared" si="49"/>
         <v>8.99</v>
       </c>
-      <c r="Q83" s="120"/>
-      <c r="R83" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S83" s="123" t="s">
+      <c r="Q83" s="105"/>
+      <c r="R83" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S83" s="108" t="s">
         <v>553</v>
       </c>
-      <c r="T83" s="124" t="s">
+      <c r="T83" s="109" t="s">
         <v>553</v>
       </c>
     </row>
@@ -9991,245 +10016,245 @@
       </c>
     </row>
     <row r="88" spans="1:20" ht="30">
-      <c r="A88" s="116" t="s">
+      <c r="A88" s="101" t="s">
         <v>544</v>
       </c>
-      <c r="B88" s="117">
-        <v>1</v>
-      </c>
-      <c r="C88" s="117" t="s">
+      <c r="B88" s="106">
+        <v>1</v>
+      </c>
+      <c r="C88" s="106" t="s">
         <v>313</v>
       </c>
-      <c r="D88" s="117" t="s">
+      <c r="D88" s="106" t="s">
         <v>383</v>
       </c>
-      <c r="E88" s="118"/>
-      <c r="F88" s="118"/>
-      <c r="G88" s="118"/>
-      <c r="H88" s="119" t="str">
+      <c r="E88" s="111"/>
+      <c r="F88" s="111"/>
+      <c r="G88" s="111"/>
+      <c r="H88" s="112" t="str">
         <f t="shared" si="48"/>
         <v>MODIFI3D - PRO 3D Print Finishing and Repair Tool</v>
       </c>
-      <c r="I88" s="120" t="s">
+      <c r="I88" s="105" t="s">
         <v>545</v>
       </c>
-      <c r="J88" s="117">
+      <c r="J88" s="106">
         <f t="shared" si="45"/>
         <v>1</v>
       </c>
-      <c r="K88" s="121"/>
-      <c r="L88" s="121">
+      <c r="K88" s="107"/>
+      <c r="L88" s="107">
         <v>89.99</v>
       </c>
-      <c r="M88" s="121">
-        <v>0</v>
-      </c>
-      <c r="N88" s="121">
-        <v>0</v>
-      </c>
-      <c r="O88" s="121">
+      <c r="M88" s="107">
+        <v>0</v>
+      </c>
+      <c r="N88" s="107">
+        <v>0</v>
+      </c>
+      <c r="O88" s="107">
         <f t="shared" si="47"/>
         <v>89.99</v>
       </c>
-      <c r="P88" s="121">
+      <c r="P88" s="107">
         <f t="shared" si="49"/>
         <v>89.99</v>
       </c>
-      <c r="Q88" s="122">
+      <c r="Q88" s="114">
         <f>-1*P88</f>
         <v>-89.99</v>
       </c>
-      <c r="R88" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S88" s="123" t="s">
+      <c r="R88" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S88" s="108" t="s">
         <v>546</v>
       </c>
-      <c r="T88" s="124" t="s">
+      <c r="T88" s="109" t="s">
         <v>547</v>
       </c>
     </row>
     <row r="89" spans="1:20" ht="30">
-      <c r="A89" s="116" t="s">
+      <c r="A89" s="101" t="s">
         <v>548</v>
       </c>
-      <c r="B89" s="117">
+      <c r="B89" s="106">
         <v>4</v>
       </c>
-      <c r="C89" s="117" t="s">
+      <c r="C89" s="106" t="s">
         <v>313</v>
       </c>
-      <c r="D89" s="117" t="s">
+      <c r="D89" s="106" t="s">
         <v>298</v>
       </c>
-      <c r="E89" s="118"/>
-      <c r="F89" s="118"/>
-      <c r="G89" s="118"/>
-      <c r="H89" s="119" t="str">
+      <c r="E89" s="111"/>
+      <c r="F89" s="111"/>
+      <c r="G89" s="111"/>
+      <c r="H89" s="112" t="str">
         <f t="shared" si="48"/>
         <v>SK6812 RGBW 5v LED (Similar to NeoPixel)</v>
       </c>
-      <c r="I89" s="120" t="s">
+      <c r="I89" s="105" t="s">
         <v>499</v>
       </c>
-      <c r="J89" s="117">
+      <c r="J89" s="106">
         <f>B89</f>
         <v>4</v>
       </c>
-      <c r="K89" s="121">
+      <c r="K89" s="107">
         <v>1.29</v>
       </c>
-      <c r="L89" s="121">
+      <c r="L89" s="107">
         <f t="shared" si="41"/>
         <v>5.16</v>
       </c>
-      <c r="M89" s="121">
-        <v>0</v>
-      </c>
-      <c r="N89" s="121">
-        <v>0</v>
-      </c>
-      <c r="O89" s="121">
+      <c r="M89" s="107">
+        <v>0</v>
+      </c>
+      <c r="N89" s="107">
+        <v>0</v>
+      </c>
+      <c r="O89" s="107">
         <f t="shared" si="42"/>
         <v>5.16</v>
       </c>
-      <c r="P89" s="121">
+      <c r="P89" s="107">
         <f t="shared" si="49"/>
         <v>5.16</v>
       </c>
-      <c r="Q89" s="122"/>
-      <c r="R89" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S89" s="123" t="s">
+      <c r="Q89" s="114"/>
+      <c r="R89" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S89" s="108" t="s">
         <v>558</v>
       </c>
-      <c r="T89" s="124" t="s">
+      <c r="T89" s="109" t="s">
         <v>552</v>
       </c>
     </row>
     <row r="90" spans="1:20" ht="30">
-      <c r="A90" s="137" t="s">
+      <c r="A90" s="136" t="s">
         <v>617</v>
       </c>
-      <c r="B90" s="117">
-        <v>1</v>
-      </c>
-      <c r="C90" s="117" t="s">
+      <c r="B90" s="106">
+        <v>1</v>
+      </c>
+      <c r="C90" s="106" t="s">
         <v>313</v>
       </c>
-      <c r="D90" s="117" t="s">
+      <c r="D90" s="106" t="s">
         <v>298</v>
       </c>
-      <c r="E90" s="118"/>
-      <c r="F90" s="118"/>
-      <c r="G90" s="118"/>
-      <c r="H90" s="119" t="str">
+      <c r="E90" s="111"/>
+      <c r="F90" s="111"/>
+      <c r="G90" s="111"/>
+      <c r="H90" s="112" t="str">
         <f t="shared" ref="H90:H94" si="53">A90</f>
         <v>LBY 100pcs Binding Screw kit,M5 x 10/20/30/40/50; Nickel Plated (Black)</v>
       </c>
-      <c r="I90" s="120" t="s">
+      <c r="I90" s="105" t="s">
         <v>611</v>
       </c>
-      <c r="J90" s="117">
+      <c r="J90" s="106">
         <f>B90</f>
         <v>1</v>
       </c>
-      <c r="K90" s="121">
+      <c r="K90" s="107">
         <v>9.19</v>
       </c>
-      <c r="L90" s="121">
+      <c r="L90" s="107">
         <f t="shared" si="41"/>
         <v>9.19</v>
       </c>
-      <c r="M90" s="121">
-        <v>0</v>
-      </c>
-      <c r="N90" s="121">
+      <c r="M90" s="107">
+        <v>0</v>
+      </c>
+      <c r="N90" s="107">
         <f>1.3/2</f>
         <v>0.65</v>
       </c>
-      <c r="O90" s="121">
+      <c r="O90" s="107">
         <f t="shared" si="42"/>
         <v>9.84</v>
       </c>
-      <c r="P90" s="121">
+      <c r="P90" s="107">
         <f t="shared" si="49"/>
         <v>9.84</v>
       </c>
-      <c r="Q90" s="120"/>
-      <c r="R90" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S90" s="123" t="s">
+      <c r="Q90" s="105"/>
+      <c r="R90" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S90" s="108" t="s">
         <v>622</v>
       </c>
-      <c r="T90" s="124" t="s">
+      <c r="T90" s="109" t="s">
         <v>618</v>
       </c>
     </row>
     <row r="91" spans="1:20">
-      <c r="A91" s="137" t="s">
+      <c r="A91" s="136" t="s">
         <v>616</v>
       </c>
-      <c r="B91" s="117">
-        <v>1</v>
-      </c>
-      <c r="C91" s="117" t="s">
+      <c r="B91" s="106">
+        <v>1</v>
+      </c>
+      <c r="C91" s="106" t="s">
         <v>313</v>
       </c>
-      <c r="D91" s="117" t="s">
+      <c r="D91" s="106" t="s">
         <v>298</v>
       </c>
-      <c r="E91" s="118"/>
-      <c r="F91" s="118"/>
-      <c r="G91" s="118"/>
-      <c r="H91" s="119" t="str">
+      <c r="E91" s="111"/>
+      <c r="F91" s="111"/>
+      <c r="G91" s="111"/>
+      <c r="H91" s="112" t="str">
         <f t="shared" si="53"/>
         <v>uxcell 10pcs Sleeve Bearing 5x7x8mm</v>
       </c>
-      <c r="I91" s="120" t="s">
+      <c r="I91" s="105" t="s">
         <v>611</v>
       </c>
-      <c r="J91" s="117">
+      <c r="J91" s="106">
         <f t="shared" ref="J91:J117" si="54">B91</f>
         <v>1</v>
       </c>
-      <c r="K91" s="121">
+      <c r="K91" s="107">
         <v>6.99</v>
       </c>
-      <c r="L91" s="121">
+      <c r="L91" s="107">
         <f t="shared" ref="L91:L117" si="55">J91*K91</f>
         <v>6.99</v>
       </c>
-      <c r="M91" s="121">
-        <v>0</v>
-      </c>
-      <c r="N91" s="121">
+      <c r="M91" s="107">
+        <v>0</v>
+      </c>
+      <c r="N91" s="107">
         <f>1.3/2</f>
         <v>0.65</v>
       </c>
-      <c r="O91" s="121">
+      <c r="O91" s="107">
         <f t="shared" ref="O91:O117" si="56">L91+M91+N91</f>
         <v>7.6400000000000006</v>
       </c>
-      <c r="P91" s="121">
+      <c r="P91" s="107">
         <f t="shared" si="49"/>
         <v>7.6400000000000006</v>
       </c>
-      <c r="Q91" s="120"/>
-      <c r="R91" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S91" s="123" t="s">
+      <c r="Q91" s="105"/>
+      <c r="R91" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S91" s="108" t="s">
         <v>619</v>
       </c>
-      <c r="T91" s="124" t="s">
+      <c r="T91" s="109" t="s">
         <v>619</v>
       </c>
     </row>
     <row r="92" spans="1:20" ht="30">
-      <c r="A92" s="154" t="s">
+      <c r="A92" s="136" t="s">
         <v>559</v>
       </c>
       <c r="B92" s="106">
@@ -10289,7 +10314,7 @@
       </c>
     </row>
     <row r="93" spans="1:20">
-      <c r="A93" s="154" t="s">
+      <c r="A93" s="136" t="s">
         <v>563</v>
       </c>
       <c r="B93" s="106">
@@ -10349,7 +10374,7 @@
       </c>
     </row>
     <row r="94" spans="1:20">
-      <c r="A94" s="154" t="s">
+      <c r="A94" s="136" t="s">
         <v>564</v>
       </c>
       <c r="B94" s="106">
@@ -10409,7 +10434,7 @@
       </c>
     </row>
     <row r="95" spans="1:20" ht="30">
-      <c r="A95" s="154" t="s">
+      <c r="A95" s="136" t="s">
         <v>607</v>
       </c>
       <c r="B95" s="106">
@@ -10435,7 +10460,7 @@
         <f t="shared" si="54"/>
         <v>8</v>
       </c>
-      <c r="K95" s="155">
+      <c r="K95" s="137">
         <v>0.12</v>
       </c>
       <c r="L95" s="107">
@@ -10470,7 +10495,7 @@
       </c>
     </row>
     <row r="96" spans="1:20">
-      <c r="A96" s="154" t="s">
+      <c r="A96" s="136" t="s">
         <v>606</v>
       </c>
       <c r="B96" s="106">
@@ -10496,7 +10521,7 @@
         <f t="shared" si="54"/>
         <v>8</v>
       </c>
-      <c r="K96" s="155">
+      <c r="K96" s="137">
         <v>0.11</v>
       </c>
       <c r="L96" s="107">
@@ -10531,7 +10556,7 @@
       </c>
     </row>
     <row r="97" spans="1:20">
-      <c r="A97" s="154" t="s">
+      <c r="A97" s="136" t="s">
         <v>608</v>
       </c>
       <c r="B97" s="106">
@@ -10557,7 +10582,7 @@
         <f t="shared" si="54"/>
         <v>12</v>
       </c>
-      <c r="K97" s="155">
+      <c r="K97" s="137">
         <v>0.2</v>
       </c>
       <c r="L97" s="107">
@@ -10592,7 +10617,7 @@
       </c>
     </row>
     <row r="98" spans="1:20" ht="30">
-      <c r="A98" s="154" t="s">
+      <c r="A98" s="136" t="s">
         <v>609</v>
       </c>
       <c r="B98" s="106">
@@ -10618,7 +10643,7 @@
         <f t="shared" si="54"/>
         <v>8</v>
       </c>
-      <c r="K98" s="155">
+      <c r="K98" s="137">
         <v>0.13</v>
       </c>
       <c r="L98" s="107">
@@ -10776,58 +10801,58 @@
       </c>
     </row>
     <row r="101" spans="1:20" ht="30">
-      <c r="A101" s="116" t="s">
+      <c r="A101" s="101" t="s">
         <v>663</v>
       </c>
-      <c r="B101" s="117">
-        <v>1</v>
-      </c>
-      <c r="C101" s="117" t="s">
+      <c r="B101" s="106">
+        <v>1</v>
+      </c>
+      <c r="C101" s="106" t="s">
         <v>313</v>
       </c>
-      <c r="D101" s="117" t="s">
+      <c r="D101" s="106" t="s">
         <v>298</v>
       </c>
-      <c r="E101" s="118"/>
-      <c r="F101" s="118"/>
-      <c r="G101" s="118"/>
-      <c r="H101" s="119"/>
-      <c r="I101" s="120" t="s">
+      <c r="E101" s="111"/>
+      <c r="F101" s="111"/>
+      <c r="G101" s="111"/>
+      <c r="H101" s="112"/>
+      <c r="I101" s="105" t="s">
         <v>662</v>
       </c>
-      <c r="J101" s="117">
+      <c r="J101" s="106">
         <f t="shared" si="64"/>
         <v>1</v>
       </c>
-      <c r="K101" s="121">
+      <c r="K101" s="107">
         <v>18.010000000000002</v>
       </c>
-      <c r="L101" s="121">
+      <c r="L101" s="107">
         <f t="shared" si="65"/>
         <v>18.010000000000002</v>
       </c>
-      <c r="M101" s="121">
-        <v>0</v>
-      </c>
-      <c r="N101" s="121">
+      <c r="M101" s="107">
+        <v>0</v>
+      </c>
+      <c r="N101" s="107">
         <v>1.33</v>
       </c>
-      <c r="O101" s="121">
+      <c r="O101" s="107">
         <f t="shared" si="66"/>
         <v>19.340000000000003</v>
       </c>
-      <c r="P101" s="121">
+      <c r="P101" s="107">
         <f>O101</f>
         <v>19.340000000000003</v>
       </c>
-      <c r="Q101" s="120"/>
-      <c r="R101" s="117" t="s">
-        <v>280</v>
-      </c>
-      <c r="S101" s="123" t="s">
+      <c r="Q101" s="105"/>
+      <c r="R101" s="106" t="s">
+        <v>392</v>
+      </c>
+      <c r="S101" s="108" t="s">
         <v>660</v>
       </c>
-      <c r="T101" s="124" t="s">
+      <c r="T101" s="109" t="s">
         <v>661</v>
       </c>
     </row>
@@ -11798,7 +11823,7 @@
       <c r="K133" s="76"/>
       <c r="L133" s="76">
         <f t="shared" ref="L133:Q133" si="67">SUM(L3:L131)</f>
-        <v>2997.3399999999983</v>
+        <v>2993.3399999999983</v>
       </c>
       <c r="M133" s="76">
         <f t="shared" si="67"/>
@@ -11810,11 +11835,11 @@
       </c>
       <c r="O133" s="76">
         <f t="shared" si="67"/>
-        <v>3233.9199999999973</v>
+        <v>3229.9199999999973</v>
       </c>
       <c r="P133" s="76">
         <f t="shared" si="67"/>
-        <v>3169.0399999999991</v>
+        <v>3166.0499999999993</v>
       </c>
       <c r="Q133" s="76">
         <f t="shared" si="67"/>
@@ -11844,7 +11869,7 @@
       </c>
       <c r="R134" s="64">
         <f>O133-P133+Q133</f>
-        <v>-300.69416666666837</v>
+        <v>-301.70416666666858</v>
       </c>
     </row>
     <row r="135" spans="1:20">
@@ -11869,7 +11894,7 @@
       </c>
       <c r="R135" s="64">
         <f>P133</f>
-        <v>3169.0399999999991</v>
+        <v>3166.0499999999993</v>
       </c>
     </row>
     <row r="136" spans="1:20">
@@ -12198,18 +12223,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21">
-      <c r="A1" s="152" t="s">
+      <c r="A1" s="151" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
-      <c r="H1" s="152"/>
-      <c r="I1" s="152"/>
-      <c r="J1" s="152"/>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="151"/>
+      <c r="I1" s="151"/>
+      <c r="J1" s="151"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" ht="19">
       <c r="A2" s="3" t="s">
@@ -12326,29 +12351,29 @@
     <col min="8" max="8" width="170" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="135" customFormat="1">
-      <c r="A1" s="135" t="s">
+    <row r="1" spans="1:8" s="133" customFormat="1">
+      <c r="A1" s="133" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="133" t="s">
         <v>294</v>
       </c>
-      <c r="C1" s="136" t="s">
+      <c r="C1" s="134" t="s">
         <v>560</v>
       </c>
-      <c r="D1" s="136" t="s">
+      <c r="D1" s="134" t="s">
         <v>605</v>
       </c>
-      <c r="E1" s="135" t="s">
+      <c r="E1" s="133" t="s">
         <v>127</v>
       </c>
-      <c r="F1" s="135" t="s">
+      <c r="F1" s="133" t="s">
         <v>572</v>
       </c>
-      <c r="G1" s="135" t="s">
+      <c r="G1" s="133" t="s">
         <v>141</v>
       </c>
-      <c r="H1" s="135" t="s">
+      <c r="H1" s="133" t="s">
         <v>3</v>
       </c>
     </row>
@@ -12556,16 +12581,16 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="19">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="152" t="s">
         <v>583</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
+      <c r="B16" s="152"/>
+      <c r="C16" s="152"/>
+      <c r="D16" s="152"/>
+      <c r="E16" s="152"/>
+      <c r="F16" s="152"/>
+      <c r="G16" s="152"/>
+      <c r="H16" s="152"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
@@ -12708,16 +12733,16 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="19">
-      <c r="A27" s="153" t="s">
+      <c r="A27" s="152" t="s">
         <v>601</v>
       </c>
-      <c r="B27" s="153"/>
-      <c r="C27" s="153"/>
-      <c r="D27" s="153"/>
-      <c r="E27" s="153"/>
-      <c r="F27" s="153"/>
-      <c r="G27" s="153"/>
-      <c r="H27" s="153"/>
+      <c r="B27" s="152"/>
+      <c r="C27" s="152"/>
+      <c r="D27" s="152"/>
+      <c r="E27" s="152"/>
+      <c r="F27" s="152"/>
+      <c r="G27" s="152"/>
+      <c r="H27" s="152"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
@@ -12916,28 +12941,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="24" customHeight="1">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="138" t="s">
         <v>293</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="139"/>
-      <c r="L1" s="139"/>
-      <c r="M1" s="139"/>
-      <c r="N1" s="139"/>
-      <c r="O1" s="139"/>
-      <c r="P1" s="139"/>
-      <c r="Q1" s="139"/>
-      <c r="R1" s="139"/>
-      <c r="S1" s="139"/>
-      <c r="T1" s="139"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
+      <c r="K1" s="138"/>
+      <c r="L1" s="138"/>
+      <c r="M1" s="138"/>
+      <c r="N1" s="138"/>
+      <c r="O1" s="138"/>
+      <c r="P1" s="138"/>
+      <c r="Q1" s="138"/>
+      <c r="R1" s="138"/>
+      <c r="S1" s="138"/>
+      <c r="T1" s="138"/>
     </row>
     <row r="2" spans="1:20" s="90" customFormat="1" ht="23" customHeight="1">
       <c r="A2" s="91" t="s">
@@ -14880,28 +14905,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="24" customHeight="1">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="138" t="s">
         <v>293</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="139"/>
-      <c r="L1" s="139"/>
-      <c r="M1" s="139"/>
-      <c r="N1" s="139"/>
-      <c r="O1" s="139"/>
-      <c r="P1" s="139"/>
-      <c r="Q1" s="139"/>
-      <c r="R1" s="139"/>
-      <c r="S1" s="139"/>
-      <c r="T1" s="139"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
+      <c r="K1" s="138"/>
+      <c r="L1" s="138"/>
+      <c r="M1" s="138"/>
+      <c r="N1" s="138"/>
+      <c r="O1" s="138"/>
+      <c r="P1" s="138"/>
+      <c r="Q1" s="138"/>
+      <c r="R1" s="138"/>
+      <c r="S1" s="138"/>
+      <c r="T1" s="138"/>
     </row>
     <row r="2" spans="1:20" s="90" customFormat="1" ht="23" customHeight="1">
       <c r="A2" s="91" t="s">
@@ -19337,24 +19362,24 @@
       </c>
     </row>
     <row r="73" spans="1:16" ht="17" thickBot="1">
-      <c r="A73" s="140" t="s">
+      <c r="A73" s="139" t="s">
         <v>288</v>
       </c>
-      <c r="B73" s="141"/>
-      <c r="C73" s="141"/>
-      <c r="D73" s="141"/>
-      <c r="E73" s="141"/>
-      <c r="F73" s="141"/>
-      <c r="G73" s="141"/>
-      <c r="H73" s="141"/>
-      <c r="I73" s="141"/>
-      <c r="J73" s="141"/>
-      <c r="K73" s="141"/>
-      <c r="L73" s="141"/>
-      <c r="M73" s="141"/>
-      <c r="N73" s="141"/>
-      <c r="O73" s="141"/>
-      <c r="P73" s="142"/>
+      <c r="B73" s="140"/>
+      <c r="C73" s="140"/>
+      <c r="D73" s="140"/>
+      <c r="E73" s="140"/>
+      <c r="F73" s="140"/>
+      <c r="G73" s="140"/>
+      <c r="H73" s="140"/>
+      <c r="I73" s="140"/>
+      <c r="J73" s="140"/>
+      <c r="K73" s="140"/>
+      <c r="L73" s="140"/>
+      <c r="M73" s="140"/>
+      <c r="N73" s="140"/>
+      <c r="O73" s="140"/>
+      <c r="P73" s="141"/>
     </row>
     <row r="74" spans="1:16" ht="17">
       <c r="A74" s="13" t="s">
@@ -19562,24 +19587,24 @@
     </row>
     <row r="85" spans="1:16" ht="17" thickBot="1"/>
     <row r="86" spans="1:16" ht="17" thickBot="1">
-      <c r="A86" s="143" t="s">
+      <c r="A86" s="142" t="s">
         <v>208</v>
       </c>
-      <c r="B86" s="144"/>
-      <c r="C86" s="144"/>
-      <c r="D86" s="144"/>
-      <c r="E86" s="144"/>
-      <c r="F86" s="144"/>
-      <c r="G86" s="144"/>
-      <c r="H86" s="144"/>
-      <c r="I86" s="144"/>
-      <c r="J86" s="144"/>
-      <c r="K86" s="144"/>
-      <c r="L86" s="144"/>
-      <c r="M86" s="144"/>
-      <c r="N86" s="144"/>
-      <c r="O86" s="144"/>
-      <c r="P86" s="145"/>
+      <c r="B86" s="143"/>
+      <c r="C86" s="143"/>
+      <c r="D86" s="143"/>
+      <c r="E86" s="143"/>
+      <c r="F86" s="143"/>
+      <c r="G86" s="143"/>
+      <c r="H86" s="143"/>
+      <c r="I86" s="143"/>
+      <c r="J86" s="143"/>
+      <c r="K86" s="143"/>
+      <c r="L86" s="143"/>
+      <c r="M86" s="143"/>
+      <c r="N86" s="143"/>
+      <c r="O86" s="143"/>
+      <c r="P86" s="144"/>
     </row>
     <row r="87" spans="1:16" ht="17">
       <c r="A87" s="13" t="s">
@@ -20002,10 +20027,10 @@
     </row>
     <row r="104" spans="1:16" ht="17" thickBot="1"/>
     <row r="105" spans="1:16" ht="17" thickTop="1">
-      <c r="A105" s="146" t="s">
+      <c r="A105" s="145" t="s">
         <v>205</v>
       </c>
-      <c r="B105" s="147"/>
+      <c r="B105" s="146"/>
       <c r="C105" s="24"/>
       <c r="D105" s="25"/>
       <c r="E105" s="26"/>
@@ -20022,8 +20047,8 @@
       <c r="P105" s="28"/>
     </row>
     <row r="106" spans="1:16" ht="17" thickBot="1">
-      <c r="A106" s="148"/>
-      <c r="B106" s="149"/>
+      <c r="A106" s="147"/>
+      <c r="B106" s="148"/>
       <c r="C106" s="30"/>
       <c r="D106" s="31"/>
       <c r="E106" s="32"/>
@@ -22373,24 +22398,24 @@
       </c>
     </row>
     <row r="73" spans="1:16" ht="17" thickBot="1">
-      <c r="A73" s="140" t="s">
+      <c r="A73" s="139" t="s">
         <v>288</v>
       </c>
-      <c r="B73" s="141"/>
-      <c r="C73" s="141"/>
-      <c r="D73" s="141"/>
-      <c r="E73" s="141"/>
-      <c r="F73" s="141"/>
-      <c r="G73" s="141"/>
-      <c r="H73" s="141"/>
-      <c r="I73" s="141"/>
-      <c r="J73" s="141"/>
-      <c r="K73" s="141"/>
-      <c r="L73" s="141"/>
-      <c r="M73" s="141"/>
-      <c r="N73" s="141"/>
-      <c r="O73" s="141"/>
-      <c r="P73" s="142"/>
+      <c r="B73" s="140"/>
+      <c r="C73" s="140"/>
+      <c r="D73" s="140"/>
+      <c r="E73" s="140"/>
+      <c r="F73" s="140"/>
+      <c r="G73" s="140"/>
+      <c r="H73" s="140"/>
+      <c r="I73" s="140"/>
+      <c r="J73" s="140"/>
+      <c r="K73" s="140"/>
+      <c r="L73" s="140"/>
+      <c r="M73" s="140"/>
+      <c r="N73" s="140"/>
+      <c r="O73" s="140"/>
+      <c r="P73" s="141"/>
     </row>
     <row r="74" spans="1:16" ht="17">
       <c r="A74" s="13" t="s">
@@ -22598,24 +22623,24 @@
     </row>
     <row r="85" spans="1:16" ht="17" thickBot="1"/>
     <row r="86" spans="1:16" ht="17" thickBot="1">
-      <c r="A86" s="143" t="s">
+      <c r="A86" s="142" t="s">
         <v>208</v>
       </c>
-      <c r="B86" s="144"/>
-      <c r="C86" s="144"/>
-      <c r="D86" s="144"/>
-      <c r="E86" s="144"/>
-      <c r="F86" s="144"/>
-      <c r="G86" s="144"/>
-      <c r="H86" s="144"/>
-      <c r="I86" s="144"/>
-      <c r="J86" s="144"/>
-      <c r="K86" s="144"/>
-      <c r="L86" s="144"/>
-      <c r="M86" s="144"/>
-      <c r="N86" s="144"/>
-      <c r="O86" s="144"/>
-      <c r="P86" s="145"/>
+      <c r="B86" s="143"/>
+      <c r="C86" s="143"/>
+      <c r="D86" s="143"/>
+      <c r="E86" s="143"/>
+      <c r="F86" s="143"/>
+      <c r="G86" s="143"/>
+      <c r="H86" s="143"/>
+      <c r="I86" s="143"/>
+      <c r="J86" s="143"/>
+      <c r="K86" s="143"/>
+      <c r="L86" s="143"/>
+      <c r="M86" s="143"/>
+      <c r="N86" s="143"/>
+      <c r="O86" s="143"/>
+      <c r="P86" s="144"/>
     </row>
     <row r="87" spans="1:16" ht="17">
       <c r="A87" s="13" t="s">
@@ -23038,10 +23063,10 @@
     </row>
     <row r="104" spans="1:16" ht="17" thickBot="1"/>
     <row r="105" spans="1:16" ht="17" thickTop="1">
-      <c r="A105" s="146" t="s">
+      <c r="A105" s="145" t="s">
         <v>205</v>
       </c>
-      <c r="B105" s="147"/>
+      <c r="B105" s="146"/>
       <c r="C105" s="24"/>
       <c r="D105" s="25"/>
       <c r="E105" s="26"/>
@@ -23058,8 +23083,8 @@
       <c r="P105" s="28"/>
     </row>
     <row r="106" spans="1:16" ht="17" thickBot="1">
-      <c r="A106" s="148"/>
-      <c r="B106" s="149"/>
+      <c r="A106" s="147"/>
+      <c r="B106" s="148"/>
       <c r="C106" s="30"/>
       <c r="D106" s="31"/>
       <c r="E106" s="32"/>
@@ -26997,10 +27022,10 @@
         <f>voron2.4_350mm_bom!M1</f>
         <v>Notes</v>
       </c>
-      <c r="Q1" s="150" t="s">
+      <c r="Q1" s="149" t="s">
         <v>135</v>
       </c>
-      <c r="R1" s="151"/>
+      <c r="R1" s="150"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="str">

</xml_diff>